<commit_message>
oppdatert deskriptives med rett antall deltagere
</commit_message>
<xml_diff>
--- a/data/Revidert_resultatskjema.xlsx
+++ b/data/Revidert_resultatskjema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3516" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{236740C1-41E5-4D67-A550-51605F6EE265}"/>
+  <xr:revisionPtr revIDLastSave="3518" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC9540BA-DFD0-4B36-A394-2F676E85D54C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,7 +749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -777,6 +777,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1161,9 +1167,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BZ9" sqref="BZ9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19284,6 +19290,7 @@
       <c r="T77" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
lagt til prosent på droppoutene
</commit_message>
<xml_diff>
--- a/data/Revidert_resultatskjema.xlsx
+++ b/data/Revidert_resultatskjema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3545" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BF55B29-EF24-4E17-9A77-38EF70A33CE7}"/>
+  <xr:revisionPtr revIDLastSave="3890" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC3697FF-2662-4DED-B773-5B68D158ED6C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,7 +785,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +795,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -851,6 +857,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1167,9 +1193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD35" sqref="AD35"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BX73" sqref="BX73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19268,1773 +19294,1892 @@
         <v>968</v>
       </c>
     </row>
-    <row r="71" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="8" t="s">
+    <row r="71" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="22">
         <v>1</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71" s="23">
         <v>61</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="24">
         <v>36.4</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="22">
         <v>168</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="22">
         <v>86</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="22">
         <v>161</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="22">
         <v>91</v>
       </c>
-      <c r="K71" s="5">
+      <c r="K71" s="23">
         <f t="shared" si="22"/>
         <v>164.5</v>
       </c>
-      <c r="L71" s="5">
+      <c r="L71" s="23">
         <f t="shared" si="23"/>
         <v>88.5</v>
       </c>
-      <c r="M71" s="4">
+      <c r="M71" s="24">
         <v>166.4</v>
       </c>
-      <c r="N71" s="4">
-        <v>102.2</v>
-      </c>
-      <c r="O71" s="4">
+      <c r="N71" s="24">
+        <f>102.2*(1+0.19%)</f>
+        <v>102.39418000000001</v>
+      </c>
+      <c r="O71" s="24">
         <v>120.5</v>
       </c>
-      <c r="P71" s="4">
+      <c r="P71" s="24">
         <v>121.5</v>
       </c>
-      <c r="Q71" s="4">
+      <c r="Q71" s="24">
         <f t="shared" si="20"/>
         <v>121</v>
       </c>
-      <c r="R71" s="5">
+      <c r="R71" s="23">
         <v>21</v>
       </c>
-      <c r="S71">
+      <c r="S71" s="22">
         <v>5.8</v>
       </c>
-      <c r="T71" s="7" t="s">
+      <c r="T71" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="U71" s="4">
+      <c r="U71" s="24">
         <v>3</v>
       </c>
-      <c r="V71" s="4">
+      <c r="V71" s="24">
         <v>3</v>
       </c>
-      <c r="W71" s="4">
+      <c r="W71" s="24">
         <v>-35</v>
       </c>
-      <c r="X71" s="4">
+      <c r="X71" s="24">
         <v>-34</v>
       </c>
-      <c r="Y71" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z71" s="4">
+      <c r="Y71" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z71" s="24">
         <v>2004</v>
       </c>
-      <c r="AA71" s="4">
+      <c r="AA71" s="24">
         <v>2005</v>
       </c>
-      <c r="AB71" s="4">
-        <v>2037.5</v>
-      </c>
-      <c r="AC71" s="4">
+      <c r="AB71" s="24">
+        <f>2037.5*(1+2.5%)</f>
+        <v>2088.4375</v>
+      </c>
+      <c r="AC71" s="24">
         <f t="shared" si="24"/>
-        <v>19.608610567514678</v>
-      </c>
-      <c r="AD71" s="4">
+        <v>19.571424860280143</v>
+      </c>
+      <c r="AD71" s="24">
         <f t="shared" si="21"/>
-        <v>19.61839530332681</v>
-      </c>
-      <c r="AE71" s="4">
+        <v>19.581191040350145</v>
+      </c>
+      <c r="AE71" s="24">
         <f t="shared" si="29"/>
-        <v>19.936399217221133</v>
-      </c>
-      <c r="AF71" s="4">
+        <v>20.396056689940774</v>
+      </c>
+      <c r="AF71" s="24">
         <f t="shared" si="25"/>
-        <v>12.5</v>
-      </c>
-      <c r="AG71" s="5">
-        <f>8.5*60</f>
-        <v>510</v>
-      </c>
-      <c r="AH71">
+        <v>12.956315097583174</v>
+      </c>
+      <c r="AG71" s="23">
+        <f>8.5*60*(1+0.81%)</f>
+        <v>514.13099999999997</v>
+      </c>
+      <c r="AH71" s="22">
         <v>3.8</v>
       </c>
-      <c r="AI71">
+      <c r="AI71" s="22">
         <v>14</v>
       </c>
-      <c r="AJ71">
+      <c r="AJ71" s="22">
         <v>17</v>
       </c>
-      <c r="AK71">
-        <v>163</v>
-      </c>
-      <c r="AL71" s="5">
+      <c r="AK71" s="22">
+        <f>163*(1-1.11%)</f>
+        <v>161.19069999999999</v>
+      </c>
+      <c r="AL71" s="23">
         <v>1954.8333333333333</v>
       </c>
-      <c r="AM71" s="4">
-        <v>58.666666666666664</v>
-      </c>
-      <c r="AN71" s="1">
-        <v>0.98999999999999988</v>
-      </c>
-      <c r="AO71" s="5">
-        <v>36.199999999999996</v>
-      </c>
-      <c r="AP71" s="1">
-        <v>5.38</v>
-      </c>
-      <c r="AQ71" s="4">
+      <c r="AM71" s="24">
+        <f>58.6666666666667*(-0.303%)+58.6666666666667</f>
+        <v>58.488906666666701</v>
+      </c>
+      <c r="AN71" s="26">
+        <f>0.99*(1-1.34%)</f>
+        <v>0.97673399999999999</v>
+      </c>
+      <c r="AO71" s="23">
+        <f>36.2*(1-3.8%)</f>
+        <v>34.824400000000004</v>
+      </c>
+      <c r="AP71" s="26">
+        <f>5.38*(1-6.6%)</f>
+        <v>5.0249199999999998</v>
+      </c>
+      <c r="AQ71" s="24">
         <v>3</v>
       </c>
-      <c r="AR71" s="1">
+      <c r="AR71" s="26">
         <f t="shared" si="26"/>
-        <v>13.991389432485324</v>
-      </c>
-      <c r="AS71" s="1">
+        <v>13.643664512963531</v>
+      </c>
+      <c r="AS71" s="26">
         <f t="shared" si="27"/>
-        <v>10.493542074363994</v>
-      </c>
-      <c r="AT71" s="5">
+        <v>10.232748384722647</v>
+      </c>
+      <c r="AT71" s="23">
         <f t="shared" si="28"/>
-        <v>71.317705735660851</v>
-      </c>
-      <c r="AU71" s="5">
-        <v>1429.92</v>
-      </c>
-      <c r="AV71" s="4">
+        <v>69.677398503740648</v>
+      </c>
+      <c r="AU71" s="23">
+        <f>1429.92*(1-2.3%)</f>
+        <v>1397.0318400000001</v>
+      </c>
+      <c r="AV71" s="24">
         <v>1100.24</v>
       </c>
-      <c r="AW71" s="4">
+      <c r="AW71" s="24">
         <v>37.36</v>
       </c>
-      <c r="AX71" s="1">
-        <v>0.76919999999999988</v>
-      </c>
-      <c r="AY71" s="4">
+      <c r="AX71" s="26">
+        <f>0.7692*(1+2.79%)</f>
+        <v>0.79066068</v>
+      </c>
+      <c r="AY71" s="24">
         <v>23.48</v>
       </c>
-      <c r="AZ71" s="4">
+      <c r="AZ71" s="24">
         <f t="shared" si="30"/>
-        <v>77.668711656441715</v>
-      </c>
-      <c r="BA71">
-        <v>126.6</v>
-      </c>
-      <c r="BB71" s="11">
+        <v>75.980090662798787</v>
+      </c>
+      <c r="BA71" s="22">
+        <f>126.6*(1-3.26%)</f>
+        <v>122.47284000000001</v>
+      </c>
+      <c r="BB71" s="27">
         <v>100311.59</v>
       </c>
-      <c r="BC71" s="11">
-        <v>46882.907229999997</v>
-      </c>
-      <c r="BD71" s="4">
-        <v>51204.995320000002</v>
-      </c>
-      <c r="BE71" s="11">
+      <c r="BC71" s="27">
+        <f>46882.90723*(1+0.15%)</f>
+        <v>46953.231590844996</v>
+      </c>
+      <c r="BD71" s="24">
+        <f>51204.99532*(1-0.163%)</f>
+        <v>51121.5311776284</v>
+      </c>
+      <c r="BE71" s="27">
         <v>34117.10671</v>
       </c>
-      <c r="BG71" s="12">
+      <c r="BG71" s="28">
         <v>2887.6836159999998</v>
       </c>
-      <c r="BH71" s="12">
+      <c r="BH71" s="28">
         <v>3060.9446330000001</v>
       </c>
-      <c r="BI71" s="12">
+      <c r="BI71" s="28">
         <v>3092.3425299999999</v>
       </c>
-      <c r="BJ71" s="12">
+      <c r="BJ71" s="28">
         <v>3277.8830819999998</v>
       </c>
-      <c r="BK71" s="4">
+      <c r="BK71" s="24">
         <f t="shared" si="31"/>
         <v>2990.0130730000001</v>
       </c>
-      <c r="BL71" s="10">
+      <c r="BL71" s="29">
         <f t="shared" si="32"/>
         <v>3169.4138574999997</v>
       </c>
-      <c r="BM71" s="4">
+      <c r="BM71" s="24">
         <v>10</v>
       </c>
-      <c r="BN71" s="1">
+      <c r="BN71" s="26">
         <v>1.58</v>
       </c>
-      <c r="BO71" s="4">
+      <c r="BO71" s="24">
         <v>1</v>
       </c>
-      <c r="BP71" s="4">
+      <c r="BP71" s="24">
         <v>5.7</v>
       </c>
-      <c r="BQ71">
+      <c r="BQ71" s="22">
         <v>131</v>
       </c>
-      <c r="BR71">
+      <c r="BR71" s="22">
         <v>44</v>
       </c>
-      <c r="BS71">
+      <c r="BS71" s="22">
         <v>12</v>
       </c>
-      <c r="BT71">
+      <c r="BT71" s="22">
         <v>27</v>
       </c>
-      <c r="BU71">
+      <c r="BU71" s="22">
         <v>18</v>
       </c>
-      <c r="BV71" s="6">
+      <c r="BV71" s="30">
         <v>12.2</v>
       </c>
-      <c r="BW71" s="7">
-        <v>200</v>
-      </c>
-      <c r="BX71" s="7">
+      <c r="BW71" s="25">
+        <f>200*(1+0.93%)</f>
+        <v>201.86</v>
+      </c>
+      <c r="BX71" s="25">
         <v>528</v>
       </c>
-      <c r="BY71">
-        <v>269</v>
-      </c>
-      <c r="BZ71">
-        <v>1091</v>
-      </c>
-      <c r="CA71">
-        <v>318</v>
-      </c>
-      <c r="CB71">
-        <v>1237</v>
+      <c r="BY71" s="22">
+        <f>269*(1-4.38%)</f>
+        <v>257.21780000000001</v>
+      </c>
+      <c r="BZ71" s="22">
+        <f>1091*(1+6.82%)</f>
+        <v>1165.4062000000001</v>
+      </c>
+      <c r="CA71" s="22">
+        <f>318*(1-4.94%)</f>
+        <v>302.29079999999999</v>
+      </c>
+      <c r="CB71" s="22">
+        <f>1237*(1+7.13%)</f>
+        <v>1325.1980999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:80" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="8" t="s">
+    <row r="72" spans="1:80" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="22">
         <v>1</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="23">
         <v>45</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="22">
         <v>29.2</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="22">
         <v>128</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="22">
         <v>92</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="22">
         <v>120</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="22">
         <v>90</v>
       </c>
-      <c r="K72" s="5">
+      <c r="K72" s="23">
         <f t="shared" si="22"/>
         <v>124</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="22">
         <f t="shared" si="23"/>
         <v>91</v>
       </c>
-      <c r="M72" s="4">
+      <c r="M72" s="24">
         <v>171.1</v>
       </c>
-      <c r="N72" s="4">
-        <v>85.8</v>
-      </c>
-      <c r="O72" s="4">
+      <c r="N72" s="24">
+        <f>85.8*(1+0.19%)</f>
+        <v>85.96302</v>
+      </c>
+      <c r="O72" s="24">
         <v>89.3</v>
       </c>
-      <c r="P72" s="4">
+      <c r="P72" s="24">
         <v>90.8</v>
       </c>
-      <c r="Q72" s="4">
+      <c r="Q72" s="24">
         <f t="shared" si="20"/>
         <v>90.05</v>
       </c>
-      <c r="R72">
+      <c r="R72" s="22">
         <v>38</v>
       </c>
-      <c r="S72">
+      <c r="S72" s="22">
         <v>73.7</v>
       </c>
-      <c r="T72" s="7" t="s">
+      <c r="T72" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="U72" s="4">
+      <c r="U72" s="24">
         <v>17.3</v>
       </c>
-      <c r="V72" s="4">
+      <c r="V72" s="24">
         <v>17.8</v>
       </c>
-      <c r="W72" s="4">
+      <c r="W72" s="24">
         <v>6.3</v>
       </c>
-      <c r="X72" s="4">
+      <c r="X72" s="24">
         <v>2.2999999999999998</v>
       </c>
-      <c r="Y72" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z72" s="4">
+      <c r="Y72" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z72" s="24">
         <v>2729</v>
       </c>
-      <c r="AA72" s="4">
+      <c r="AA72" s="24">
         <v>2751.9166666666665</v>
       </c>
-      <c r="AB72" s="4">
-        <v>2843.8333333333335</v>
-      </c>
-      <c r="AC72" s="4">
+      <c r="AB72" s="24">
+        <f>2843.83333333333*(1+2.5%)</f>
+        <v>2914.9291666666627</v>
+      </c>
+      <c r="AC72" s="24">
         <f t="shared" si="24"/>
-        <v>31.806526806526808</v>
-      </c>
-      <c r="AD72" s="4">
+        <v>31.746209009408929</v>
+      </c>
+      <c r="AD72" s="24">
         <f t="shared" si="21"/>
-        <v>32.073620823620821</v>
-      </c>
-      <c r="AE72" s="4">
+        <v>32.012796510251341</v>
+      </c>
+      <c r="AE72" s="24">
         <f t="shared" si="29"/>
-        <v>33.144910644910645</v>
-      </c>
-      <c r="AF72" s="4">
+        <v>33.909106109425458</v>
+      </c>
+      <c r="AF72" s="24">
         <f t="shared" si="25"/>
-        <v>15.046737213403881</v>
-      </c>
-      <c r="AG72" s="5">
-        <f>12*60</f>
-        <v>720</v>
-      </c>
-      <c r="AH72">
+        <v>15.596021482191279</v>
+      </c>
+      <c r="AG72" s="23">
+        <f>12*60*(1+0.81%)</f>
+        <v>725.83199999999999</v>
+      </c>
+      <c r="AH72" s="22">
         <v>4.8</v>
       </c>
-      <c r="AI72">
+      <c r="AI72" s="22">
         <v>20</v>
       </c>
-      <c r="AJ72">
+      <c r="AJ72" s="22">
         <v>19</v>
       </c>
-      <c r="AK72">
-        <v>189</v>
-      </c>
-      <c r="AL72" s="5">
+      <c r="AK72" s="22">
+        <f>189*(1-1.11%)</f>
+        <v>186.90209999999999</v>
+      </c>
+      <c r="AL72" s="23">
         <v>3413.1666666666665</v>
       </c>
-      <c r="AM72" s="4">
-        <v>96.333333333333329</v>
-      </c>
-      <c r="AN72" s="1">
-        <v>1.2366666666666666</v>
-      </c>
-      <c r="AO72" s="5">
-        <v>42.583333333333336</v>
-      </c>
-      <c r="AP72" s="1">
-        <v>9.27</v>
-      </c>
-      <c r="AQ72" s="4">
+      <c r="AM72" s="24">
+        <f>96.3333333333333*(-0.303%)+96.3333333333333</f>
+        <v>96.041443333333305</v>
+      </c>
+      <c r="AN72" s="26">
+        <f>1.23666666666667*(1-1.34%)</f>
+        <v>1.2200953333333366</v>
+      </c>
+      <c r="AO72" s="23">
+        <f>42.5833333333333*(1-3.8%)</f>
+        <v>40.965166666666633</v>
+      </c>
+      <c r="AP72" s="26">
+        <f>9.27*(1-6.6%)</f>
+        <v>8.6581799999999998</v>
+      </c>
+      <c r="AQ72" s="24">
         <v>3.5</v>
       </c>
-      <c r="AR72" s="1">
+      <c r="AR72" s="26">
         <f t="shared" si="26"/>
-        <v>16.337529137529138</v>
-      </c>
-      <c r="AS72" s="1">
+        <v>15.931496124728984</v>
+      </c>
+      <c r="AS72" s="26">
         <f t="shared" si="27"/>
-        <v>12.253146853146854</v>
-      </c>
-      <c r="AT72" s="5">
+        <v>11.948622093546739</v>
+      </c>
+      <c r="AT72" s="23">
         <f t="shared" si="28"/>
-        <v>50.93758895315387</v>
-      </c>
-      <c r="AU72" s="5">
-        <v>1401.76</v>
-      </c>
-      <c r="AV72" s="4">
+        <v>49.766024407231328</v>
+      </c>
+      <c r="AU72" s="23">
+        <f>1401.76*(1-2.3%)</f>
+        <v>1369.5195200000001</v>
+      </c>
+      <c r="AV72" s="24">
         <v>1153.68</v>
       </c>
-      <c r="AW72" s="4">
+      <c r="AW72" s="24">
         <v>34.840000000000003</v>
       </c>
-      <c r="AX72" s="1">
-        <v>0.8248000000000002</v>
-      </c>
-      <c r="AY72" s="4">
+      <c r="AX72" s="26">
+        <f>0.8248*(1+2.79%)</f>
+        <v>0.84781192000000005</v>
+      </c>
+      <c r="AY72" s="24">
         <v>22.971999999999998</v>
       </c>
-      <c r="AZ72" s="4">
+      <c r="AZ72" s="24">
         <f t="shared" si="30"/>
-        <v>62.010582010582013</v>
-      </c>
-      <c r="BA72">
-        <v>117.2</v>
-      </c>
-      <c r="BB72" s="11">
+        <v>60.662389561165988</v>
+      </c>
+      <c r="BA72" s="22">
+        <f>117.2*(1-3.26%)</f>
+        <v>113.37928000000001</v>
+      </c>
+      <c r="BB72" s="27">
         <v>85828.390270000004</v>
       </c>
-      <c r="BC72" s="11">
-        <v>48248.861250000002</v>
-      </c>
-      <c r="BD72" s="11">
-        <v>35113.285960000001</v>
-      </c>
-      <c r="BE72" s="11">
+      <c r="BC72" s="27">
+        <f>48248.86125*(1+0.15%)</f>
+        <v>48321.234541875005</v>
+      </c>
+      <c r="BD72" s="27">
+        <f>35113.28596*(1-0.163%)</f>
+        <v>35056.0513038852</v>
+      </c>
+      <c r="BE72" s="27">
         <v>16707.703570000001</v>
       </c>
-      <c r="BG72" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BH72" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BI72" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BJ72" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK72" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BL72" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="BM72" s="4">
+      <c r="BG72" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH72" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI72" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ72" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK72" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BL72" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM72" s="24">
         <v>4.2</v>
       </c>
-      <c r="BN72" s="1">
+      <c r="BN72" s="26">
         <v>0.98</v>
       </c>
-      <c r="BO72" s="4">
+      <c r="BO72" s="24">
         <v>1.2</v>
       </c>
-      <c r="BP72" s="4">
+      <c r="BP72" s="24">
         <v>2.7</v>
       </c>
-      <c r="BQ72">
+      <c r="BQ72" s="22">
         <v>109</v>
       </c>
-      <c r="BR72">
+      <c r="BR72" s="22">
         <v>34</v>
       </c>
-      <c r="BS72">
+      <c r="BS72" s="22">
         <v>17</v>
       </c>
-      <c r="BT72">
+      <c r="BT72" s="22">
         <v>49</v>
       </c>
-      <c r="BU72">
+      <c r="BU72" s="22">
         <v>39</v>
       </c>
-      <c r="BV72" s="4">
+      <c r="BV72" s="24">
         <v>6.7</v>
       </c>
-      <c r="BW72">
-        <v>205</v>
-      </c>
-      <c r="BX72">
+      <c r="BW72" s="22">
+        <f>205*(1+0.93%)</f>
+        <v>206.90650000000002</v>
+      </c>
+      <c r="BX72" s="22">
         <v>473</v>
       </c>
-      <c r="BY72">
-        <v>345</v>
-      </c>
-      <c r="BZ72">
-        <v>1332</v>
-      </c>
-      <c r="CA72">
-        <v>341</v>
-      </c>
-      <c r="CB72">
-        <v>1275</v>
+      <c r="BY72" s="22">
+        <f>345*(1-4.38%)</f>
+        <v>329.88900000000001</v>
+      </c>
+      <c r="BZ72" s="22">
+        <f>1332*(1+6.82%)</f>
+        <v>1422.8424</v>
+      </c>
+      <c r="CA72" s="22">
+        <f>341*(1-4.94%)</f>
+        <v>324.15460000000002</v>
+      </c>
+      <c r="CB72" s="22">
+        <f>1275*(1+7.13%)</f>
+        <v>1365.9074999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="8" t="s">
+    <row r="73" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="22">
         <v>1</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="23">
         <v>66</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="24">
         <v>26.6</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="22">
         <v>161</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="22">
         <v>85</v>
       </c>
-      <c r="I73">
+      <c r="I73" s="22">
         <v>147</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="22">
         <v>79</v>
       </c>
-      <c r="K73" s="5">
+      <c r="K73" s="23">
         <f t="shared" si="22"/>
         <v>154</v>
       </c>
-      <c r="L73">
+      <c r="L73" s="22">
         <f t="shared" si="23"/>
         <v>82</v>
       </c>
-      <c r="M73" s="4">
+      <c r="M73" s="24">
         <v>168.5</v>
       </c>
-      <c r="N73" s="4">
-        <v>75.599999999999994</v>
-      </c>
-      <c r="O73" s="4">
+      <c r="N73" s="24">
+        <f>75.6*(1+0.19%)</f>
+        <v>75.743639999999999</v>
+      </c>
+      <c r="O73" s="24">
         <v>85</v>
       </c>
-      <c r="P73" s="4">
+      <c r="P73" s="24">
         <v>85</v>
       </c>
-      <c r="Q73" s="4">
+      <c r="Q73" s="24">
         <f t="shared" si="20"/>
         <v>85</v>
       </c>
-      <c r="R73" s="5">
+      <c r="R73" s="23">
         <v>21</v>
       </c>
-      <c r="S73" s="4">
+      <c r="S73" s="24">
         <v>66</v>
       </c>
-      <c r="T73" s="7" t="s">
+      <c r="T73" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="U73" s="4">
+      <c r="U73" s="24">
         <v>8</v>
       </c>
-      <c r="V73" s="4">
+      <c r="V73" s="24">
         <v>11.5</v>
       </c>
-      <c r="W73" s="4">
+      <c r="W73" s="24">
         <v>0</v>
       </c>
-      <c r="X73" s="4">
+      <c r="X73" s="24">
         <v>-12</v>
       </c>
-      <c r="Y73">
+      <c r="Y73" s="22">
         <v>12</v>
       </c>
-      <c r="Z73" s="4">
+      <c r="Z73" s="24">
         <v>1950</v>
       </c>
-      <c r="AA73" s="4">
+      <c r="AA73" s="24">
         <v>1938.25</v>
       </c>
-      <c r="AB73" s="4">
-        <v>1968.1666666666667</v>
-      </c>
-      <c r="AC73" s="4">
+      <c r="AB73" s="24">
+        <f>1968.16666666667*(1+2.5%)</f>
+        <v>2017.3708333333366</v>
+      </c>
+      <c r="AC73" s="24">
         <f t="shared" si="24"/>
-        <v>25.793650793650794</v>
-      </c>
-      <c r="AD73" s="4">
+        <v>25.74473579563908</v>
+      </c>
+      <c r="AD73" s="24">
         <f t="shared" si="21"/>
-        <v>25.638227513227516</v>
-      </c>
-      <c r="AE73" s="4">
+        <v>25.589607259434587</v>
+      </c>
+      <c r="AE73" s="24">
         <f t="shared" si="29"/>
-        <v>26.033950617283953</v>
-      </c>
-      <c r="AF73" s="4">
+        <v>26.634194413330764</v>
+      </c>
+      <c r="AF73" s="24">
         <f t="shared" si="25"/>
-        <v>11.577450980392157</v>
-      </c>
-      <c r="AG73" s="5">
-        <f>60*11+50</f>
-        <v>710</v>
-      </c>
-      <c r="AH73">
+        <v>12.000088234302741</v>
+      </c>
+      <c r="AG73" s="23">
+        <f>60*11+50*(1+0.81%)</f>
+        <v>710.40499999999997</v>
+      </c>
+      <c r="AH73" s="22">
         <v>3.8</v>
       </c>
-      <c r="AI73">
+      <c r="AI73" s="22">
         <v>18</v>
       </c>
-      <c r="AJ73">
+      <c r="AJ73" s="22">
         <v>20</v>
       </c>
-      <c r="AK73">
-        <v>170</v>
-      </c>
-      <c r="AL73" s="5">
+      <c r="AK73" s="22">
+        <f>170*(1-1.11%)</f>
+        <v>168.113</v>
+      </c>
+      <c r="AL73" s="23">
         <v>2318.3333333333335</v>
       </c>
-      <c r="AM73" s="4">
-        <v>72.333333333333329</v>
-      </c>
-      <c r="AN73" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="AO73" s="5">
-        <v>38.099999999999994</v>
-      </c>
-      <c r="AP73" s="1">
-        <v>5.7</v>
-      </c>
-      <c r="AQ73" s="4">
+      <c r="AM73" s="24">
+        <f>72.3333333333333*(-0.303%)+72.3333333333333</f>
+        <v>72.114163333333295</v>
+      </c>
+      <c r="AN73" s="26">
+        <f>1.2*(1-1.34%)</f>
+        <v>1.1839200000000001</v>
+      </c>
+      <c r="AO73" s="23">
+        <f>38.1*(1-3.8%)</f>
+        <v>36.652200000000001</v>
+      </c>
+      <c r="AP73" s="26">
+        <f>5.7*(1-6.6%)</f>
+        <v>5.3237999999999994</v>
+      </c>
+      <c r="AQ73" s="24">
         <v>3</v>
       </c>
-      <c r="AR73" s="1">
+      <c r="AR73" s="26">
         <f t="shared" si="26"/>
-        <v>14.352380952380953</v>
-      </c>
-      <c r="AS73" s="1">
+        <v>13.995684390134933</v>
+      </c>
+      <c r="AS73" s="26">
         <f t="shared" si="27"/>
-        <v>10.764285714285714</v>
-      </c>
-      <c r="AT73" s="5">
+        <v>10.4967632926012</v>
+      </c>
+      <c r="AT73" s="23">
         <f t="shared" si="28"/>
-        <v>55.980394685928026</v>
-      </c>
-      <c r="AU73" s="5">
-        <v>1085.04</v>
-      </c>
-      <c r="AV73" s="4">
+        <v>54.692845608151671</v>
+      </c>
+      <c r="AU73" s="23">
+        <f>1085.04*(1-2.3%)</f>
+        <v>1060.0840799999999</v>
+      </c>
+      <c r="AV73" s="24">
         <v>903.76</v>
       </c>
-      <c r="AW73" s="4">
+      <c r="AW73" s="24">
         <v>30.2</v>
       </c>
-      <c r="AX73" s="1">
-        <v>0.83279999999999987</v>
-      </c>
-      <c r="AY73" s="4">
+      <c r="AX73" s="26">
+        <f>0.8328*(1+2.79%)</f>
+        <v>0.85603512000000004</v>
+      </c>
+      <c r="AY73" s="24">
         <v>21.475999999999999</v>
       </c>
-      <c r="AZ73" s="4">
+      <c r="AZ73" s="24">
         <f t="shared" si="30"/>
-        <v>78.35294117647058</v>
-      </c>
-      <c r="BA73">
-        <v>133.19999999999999</v>
-      </c>
-      <c r="BB73" s="11">
+        <v>76.649444123892849</v>
+      </c>
+      <c r="BA73" s="22">
+        <f>133.2*(1-3.26%)</f>
+        <v>128.85767999999999</v>
+      </c>
+      <c r="BB73" s="27">
         <v>75715.09</v>
       </c>
-      <c r="BC73" s="11">
-        <v>41266.961259999996</v>
-      </c>
-      <c r="BD73" s="11">
-        <v>32618.593929999999</v>
-      </c>
-      <c r="BE73" s="11">
+      <c r="BC73" s="27">
+        <f>41266.96126*(1+0.15%)</f>
+        <v>41328.861701889997</v>
+      </c>
+      <c r="BD73" s="27">
+        <f>32618.59393*(1-0.163%)</f>
+        <v>32565.425621894097</v>
+      </c>
+      <c r="BE73" s="27">
         <v>16043.331039999999</v>
       </c>
-      <c r="BG73" s="12">
+      <c r="BG73" s="28">
         <v>1141.71261</v>
       </c>
-      <c r="BH73" s="12">
+      <c r="BH73" s="28">
         <v>1210.2153659999999</v>
       </c>
-      <c r="BI73" s="12">
+      <c r="BI73" s="28">
         <v>1189.3955530000001</v>
       </c>
-      <c r="BJ73" s="12">
+      <c r="BJ73" s="28">
         <v>1260.759286</v>
       </c>
-      <c r="BK73" s="4">
+      <c r="BK73" s="24">
         <f t="shared" ref="BK73:BK77" si="33">AVERAGE(BG73,BI73)</f>
         <v>1165.5540814999999</v>
       </c>
-      <c r="BL73" s="10">
+      <c r="BL73" s="29">
         <f t="shared" ref="BL73:BL77" si="34">AVERAGE(BH73,BJ73)</f>
         <v>1235.4873259999999</v>
       </c>
-      <c r="BM73" s="4">
+      <c r="BM73" s="24">
         <v>5.8</v>
       </c>
-      <c r="BN73" s="1">
+      <c r="BN73" s="26">
         <v>0.86</v>
       </c>
-      <c r="BO73" s="4">
+      <c r="BO73" s="24">
         <v>1.5</v>
       </c>
-      <c r="BP73" s="4">
+      <c r="BP73" s="24">
         <v>3.4</v>
       </c>
-      <c r="BQ73">
+      <c r="BQ73" s="22">
         <v>136</v>
       </c>
-      <c r="BR73">
+      <c r="BR73" s="22">
         <v>58</v>
       </c>
-      <c r="BS73">
+      <c r="BS73" s="22">
         <v>14</v>
       </c>
-      <c r="BT73">
+      <c r="BT73" s="22">
         <v>25</v>
       </c>
-      <c r="BU73">
+      <c r="BU73" s="22">
         <v>17</v>
       </c>
-      <c r="BV73" s="4">
+      <c r="BV73" s="24">
         <v>8.1</v>
       </c>
-      <c r="BW73">
-        <v>175</v>
-      </c>
-      <c r="BX73">
+      <c r="BW73" s="22">
+        <f>175*(1+0.93%)</f>
+        <v>176.62750000000003</v>
+      </c>
+      <c r="BX73" s="22">
         <v>171</v>
       </c>
-      <c r="BY73">
-        <v>240</v>
-      </c>
-      <c r="BZ73">
-        <v>909</v>
-      </c>
-      <c r="CA73">
-        <v>238</v>
-      </c>
-      <c r="CB73">
-        <v>910</v>
+      <c r="BY73" s="22">
+        <f>240*(1-4.38%)</f>
+        <v>229.488</v>
+      </c>
+      <c r="BZ73" s="22">
+        <f>909*(1+6.82%)</f>
+        <v>970.99380000000008</v>
+      </c>
+      <c r="CA73" s="22">
+        <f>238*(1-4.94%)</f>
+        <v>226.24279999999999</v>
+      </c>
+      <c r="CB73" s="22">
+        <f>910*(1+7.13%)</f>
+        <v>974.88299999999992</v>
       </c>
     </row>
-    <row r="74" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="8" t="s">
+    <row r="74" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="22">
         <v>2</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="23">
         <v>46</v>
       </c>
-      <c r="F74" s="4">
+      <c r="F74" s="24">
         <v>42.8</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="22">
         <v>163</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="22">
         <v>105</v>
       </c>
-      <c r="I74">
+      <c r="I74" s="22">
         <v>164</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="22">
         <v>112</v>
       </c>
-      <c r="K74" s="5">
+      <c r="K74" s="23">
         <f t="shared" si="22"/>
         <v>163.5</v>
       </c>
-      <c r="L74" s="5">
+      <c r="L74" s="23">
         <f t="shared" si="23"/>
         <v>108.5</v>
       </c>
-      <c r="M74" s="4">
+      <c r="M74" s="24">
         <v>187.6</v>
       </c>
-      <c r="N74" s="4">
-        <v>149.69999999999999</v>
-      </c>
-      <c r="O74" s="4">
+      <c r="N74" s="24">
+        <f>149.7*(1+0.19%)</f>
+        <v>149.98443</v>
+      </c>
+      <c r="O74" s="24">
         <v>146</v>
       </c>
-      <c r="P74" s="4">
+      <c r="P74" s="24">
         <v>145</v>
       </c>
-      <c r="Q74" s="4">
+      <c r="Q74" s="24">
         <f t="shared" si="20"/>
         <v>145.5</v>
       </c>
-      <c r="R74" s="5">
+      <c r="R74" s="23">
         <v>89</v>
       </c>
-      <c r="S74" s="4">
+      <c r="S74" s="24">
         <v>64</v>
       </c>
-      <c r="T74" s="7" t="s">
+      <c r="T74" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="U74" s="4">
+      <c r="U74" s="24">
         <v>-12.5</v>
       </c>
-      <c r="V74" s="4">
+      <c r="V74" s="24">
         <v>-2.5</v>
       </c>
-      <c r="W74" s="4">
+      <c r="W74" s="24">
         <v>-3.5</v>
       </c>
-      <c r="X74" s="4">
+      <c r="X74" s="24">
         <v>-3</v>
       </c>
-      <c r="Y74" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z74" s="4">
+      <c r="Y74" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z74" s="24">
         <v>3715</v>
       </c>
-      <c r="AA74" s="4">
+      <c r="AA74" s="24">
         <v>3737.4166666666665</v>
       </c>
-      <c r="AB74" s="4">
-        <v>3757</v>
-      </c>
-      <c r="AC74" s="4">
+      <c r="AB74" s="24">
+        <f>3757*(1+2.5%)</f>
+        <v>3850.9249999999997</v>
+      </c>
+      <c r="AC74" s="24">
         <f t="shared" si="24"/>
-        <v>24.816299265197063</v>
-      </c>
-      <c r="AD74" s="4">
+        <v>24.769237713541333</v>
+      </c>
+      <c r="AD74" s="24">
         <f t="shared" si="21"/>
-        <v>24.966043197506124</v>
-      </c>
-      <c r="AE74" s="4">
+        <v>24.918697671929454</v>
+      </c>
+      <c r="AE74" s="24">
         <f t="shared" si="29"/>
-        <v>25.096860387441552</v>
-      </c>
-      <c r="AF74" s="4">
+        <v>25.67549845007245</v>
+      </c>
+      <c r="AF74" s="24">
         <f t="shared" si="25"/>
-        <v>18.974747474747474</v>
-      </c>
-      <c r="AG74" s="5">
-        <f>8.5*60+5</f>
-        <v>515</v>
-      </c>
-      <c r="AH74" s="4">
+        <v>19.667424574391912</v>
+      </c>
+      <c r="AG74" s="23">
+        <f>8.5*60+5*(1+0.81%)</f>
+        <v>515.04049999999995</v>
+      </c>
+      <c r="AH74" s="24">
         <v>4.8</v>
       </c>
-      <c r="AI74">
+      <c r="AI74" s="22">
         <v>12</v>
       </c>
-      <c r="AJ74">
+      <c r="AJ74" s="22">
         <v>19</v>
       </c>
-      <c r="AK74">
-        <v>198</v>
-      </c>
-      <c r="AL74" s="5">
+      <c r="AK74" s="22">
+        <f>198*(1-1.11%)</f>
+        <v>195.8022</v>
+      </c>
+      <c r="AL74" s="23">
         <v>4427</v>
       </c>
-      <c r="AM74" s="4">
-        <v>128.5</v>
-      </c>
-      <c r="AN74" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="AO74" s="5">
-        <v>33.366666666666667</v>
-      </c>
-      <c r="AP74" s="1">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="AQ74" s="4">
+      <c r="AM74" s="24">
+        <f>128.5*(-0.303%)+128.5</f>
+        <v>128.11064500000001</v>
+      </c>
+      <c r="AN74" s="26">
+        <f>1.2*(1-1.34%)</f>
+        <v>1.1839200000000001</v>
+      </c>
+      <c r="AO74" s="23">
+        <f>33.3666666666667*(1-3.8%)</f>
+        <v>32.098733333333364</v>
+      </c>
+      <c r="AP74" s="26">
+        <f>4.64*(1-6.6%)</f>
+        <v>4.3337599999999998</v>
+      </c>
+      <c r="AQ74" s="24">
         <v>3.5</v>
       </c>
-      <c r="AR74" s="1">
+      <c r="AR74" s="26">
         <f t="shared" si="26"/>
-        <v>16.020574482297931</v>
-      </c>
-      <c r="AS74" s="1">
+        <v>15.622418673724999</v>
+      </c>
+      <c r="AS74" s="26">
         <f t="shared" si="27"/>
-        <v>12.015430861723448</v>
-      </c>
-      <c r="AT74" s="5">
+        <v>11.716814005293749</v>
+      </c>
+      <c r="AT74" s="23">
         <f t="shared" si="28"/>
-        <v>64.169457512988032</v>
-      </c>
-      <c r="AU74" s="5">
-        <v>2398.2800000000002</v>
-      </c>
-      <c r="AV74" s="4">
+        <v>62.693559990189307</v>
+      </c>
+      <c r="AU74" s="23">
+        <f>2398.28*(1-2.3%)</f>
+        <v>2343.1195600000001</v>
+      </c>
+      <c r="AV74" s="24">
         <v>1928.2</v>
       </c>
-      <c r="AW74" s="4">
+      <c r="AW74" s="24">
         <v>54.48</v>
       </c>
-      <c r="AX74" s="1">
-        <v>0.80279999999999985</v>
-      </c>
-      <c r="AY74" s="4">
+      <c r="AX74" s="26">
+        <f>0.8028*(1+2.79%)</f>
+        <v>0.82519812000000003</v>
+      </c>
+      <c r="AY74" s="24">
         <v>18.779999999999994</v>
       </c>
-      <c r="AZ74" s="4">
+      <c r="AZ74" s="24">
         <f t="shared" si="30"/>
-        <v>64.343434343434353</v>
-      </c>
-      <c r="BA74" s="4">
-        <v>127.4</v>
-      </c>
-      <c r="BB74" s="11">
+        <v>62.944522584526631</v>
+      </c>
+      <c r="BA74" s="24">
+        <f>127.4*(1-3.26%)</f>
+        <v>123.24676000000001</v>
+      </c>
+      <c r="BB74" s="27">
         <v>150206.23000000001</v>
       </c>
-      <c r="BC74" s="11">
-        <v>82789.589590000003</v>
-      </c>
-      <c r="BD74" s="11">
-        <v>64095.72913</v>
-      </c>
-      <c r="BE74" s="11">
+      <c r="BC74" s="27">
+        <f>82789.58959*(1+0.15%)</f>
+        <v>82913.773974385011</v>
+      </c>
+      <c r="BD74" s="27">
+        <f>64095.72913*(1-0.163%)</f>
+        <v>63991.253091518098</v>
+      </c>
+      <c r="BE74" s="27">
         <v>42715.55816</v>
       </c>
-      <c r="BG74" s="12">
+      <c r="BG74" s="28">
         <v>3601.528053</v>
       </c>
-      <c r="BH74" s="12">
+      <c r="BH74" s="28">
         <v>3817.6197360000001</v>
       </c>
-      <c r="BI74" s="12">
+      <c r="BI74" s="28">
         <v>3203.00614</v>
       </c>
-      <c r="BJ74" s="12">
+      <c r="BJ74" s="28">
         <v>3395.1865079999998</v>
       </c>
-      <c r="BK74" s="4">
+      <c r="BK74" s="24">
         <f t="shared" si="33"/>
         <v>3402.2670964999998</v>
       </c>
-      <c r="BL74" s="10">
+      <c r="BL74" s="29">
         <f t="shared" si="34"/>
         <v>3606.4031219999997</v>
       </c>
-      <c r="BM74" s="4">
+      <c r="BM74" s="24">
         <v>5.7</v>
       </c>
-      <c r="BN74" s="1">
+      <c r="BN74" s="26">
         <v>1.97</v>
       </c>
-      <c r="BO74" s="4">
+      <c r="BO74" s="24">
         <v>1.2</v>
       </c>
-      <c r="BP74" s="4">
+      <c r="BP74" s="24">
         <v>3.5</v>
       </c>
-      <c r="BQ74">
+      <c r="BQ74" s="22">
         <v>143</v>
       </c>
-      <c r="BR74">
+      <c r="BR74" s="22">
         <v>44</v>
       </c>
-      <c r="BS74">
+      <c r="BS74" s="22">
         <v>15</v>
       </c>
-      <c r="BT74">
+      <c r="BT74" s="22">
         <v>34</v>
       </c>
-      <c r="BU74">
+      <c r="BU74" s="22">
         <v>33</v>
       </c>
-      <c r="BV74" s="6">
+      <c r="BV74" s="30">
         <v>9.5</v>
       </c>
-      <c r="BW74" s="7">
-        <v>360</v>
-      </c>
-      <c r="BX74" s="7">
+      <c r="BW74" s="25">
+        <f>360*(1+0.93%)</f>
+        <v>363.34800000000001</v>
+      </c>
+      <c r="BX74" s="25">
         <v>378</v>
       </c>
-      <c r="BY74">
-        <v>767</v>
-      </c>
-      <c r="BZ74">
-        <v>1975</v>
-      </c>
-      <c r="CA74">
-        <v>784</v>
-      </c>
-      <c r="CB74">
-        <v>2068</v>
+      <c r="BY74" s="22">
+        <f>767*(1-4.38%)</f>
+        <v>733.40539999999999</v>
+      </c>
+      <c r="BZ74" s="22">
+        <f>1975*(1+6.82%)</f>
+        <v>2109.6950000000002</v>
+      </c>
+      <c r="CA74" s="22">
+        <f>784*(1-4.94%)</f>
+        <v>745.2704</v>
+      </c>
+      <c r="CB74" s="22">
+        <f>2068*(1+7.13%)</f>
+        <v>2215.4483999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="8" t="s">
+    <row r="75" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="22">
         <v>1</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="23">
         <v>39</v>
       </c>
-      <c r="F75" s="4">
+      <c r="F75" s="24">
         <v>41.6</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="22">
         <v>108</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="22">
         <v>70</v>
       </c>
-      <c r="I75">
+      <c r="I75" s="22">
         <v>122</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="22">
         <v>77</v>
       </c>
-      <c r="K75" s="5">
+      <c r="K75" s="23">
         <f t="shared" si="22"/>
         <v>115</v>
       </c>
-      <c r="L75" s="5">
+      <c r="L75" s="23">
         <f t="shared" si="23"/>
         <v>73.5</v>
       </c>
-      <c r="M75" s="4">
+      <c r="M75" s="24">
         <v>173.1</v>
       </c>
-      <c r="N75" s="4">
-        <v>125.5</v>
-      </c>
-      <c r="O75" s="4">
+      <c r="N75" s="24">
+        <f>125.5*(1+0.19%)</f>
+        <v>125.73845</v>
+      </c>
+      <c r="O75" s="24">
         <v>118.7</v>
       </c>
-      <c r="P75" s="4">
+      <c r="P75" s="24">
         <v>119.4</v>
       </c>
-      <c r="Q75" s="4">
+      <c r="Q75" s="24">
         <f t="shared" si="20"/>
         <v>119.05000000000001</v>
       </c>
-      <c r="R75">
+      <c r="R75" s="22">
         <v>28</v>
       </c>
-      <c r="S75">
+      <c r="S75" s="22">
         <v>31.6</v>
       </c>
-      <c r="T75" s="7" t="s">
+      <c r="T75" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="U75" s="4">
+      <c r="U75" s="24">
         <v>5.2</v>
       </c>
-      <c r="V75" s="4">
+      <c r="V75" s="24">
         <v>7.2</v>
       </c>
-      <c r="W75" s="4">
+      <c r="W75" s="24">
         <v>-16</v>
       </c>
-      <c r="X75" s="4">
+      <c r="X75" s="24">
         <v>-29.7</v>
       </c>
-      <c r="Y75" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z75" s="4">
+      <c r="Y75" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z75" s="24">
         <v>1744</v>
       </c>
-      <c r="AA75" s="4">
+      <c r="AA75" s="24">
         <v>1753.8333333333333</v>
       </c>
-      <c r="AB75" s="4">
-        <v>1858.1666666666667</v>
-      </c>
-      <c r="AC75" s="4">
+      <c r="AB75" s="24">
+        <f>1858.16666666667*(1+2.5%)</f>
+        <v>1904.6208333333366</v>
+      </c>
+      <c r="AC75" s="24">
         <f t="shared" si="24"/>
-        <v>13.896414342629482</v>
-      </c>
-      <c r="AD75" s="4">
+        <v>13.870061226299512</v>
+      </c>
+      <c r="AD75" s="24">
         <f t="shared" si="21"/>
-        <v>13.97476759628154</v>
-      </c>
-      <c r="AE75" s="4">
+        <v>13.948265891088472</v>
+      </c>
+      <c r="AE75" s="24">
         <f t="shared" si="29"/>
-        <v>14.806108897742364</v>
-      </c>
-      <c r="AF75" s="4">
+        <v>15.147481405515469</v>
+      </c>
+      <c r="AF75" s="24">
         <f t="shared" si="25"/>
-        <v>11.686582809224319</v>
-      </c>
-      <c r="AG75" s="5">
-        <f>3*60+25</f>
-        <v>205</v>
-      </c>
-      <c r="AH75">
+        <v>12.113203943224743</v>
+      </c>
+      <c r="AG75" s="23">
+        <f>3*60+25*(1+0.81%)</f>
+        <v>205.20249999999999</v>
+      </c>
+      <c r="AH75" s="22">
         <v>3.5</v>
       </c>
-      <c r="AI75">
+      <c r="AI75" s="22">
         <v>6</v>
       </c>
-      <c r="AJ75">
+      <c r="AJ75" s="22">
         <v>19</v>
       </c>
-      <c r="AK75">
-        <v>159</v>
-      </c>
-      <c r="AL75" s="5">
+      <c r="AK75" s="22">
+        <f>159*(1-1.11%)</f>
+        <v>157.23509999999999</v>
+      </c>
+      <c r="AL75" s="23">
         <v>2068.3333333333335</v>
       </c>
-      <c r="AM75" s="4">
-        <v>70.166666666666671</v>
-      </c>
-      <c r="AN75" s="1">
-        <v>1.1449999999999998</v>
-      </c>
-      <c r="AO75" s="5">
-        <v>33.283333333333331</v>
-      </c>
-      <c r="AP75" s="1">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="AQ75" s="4">
+      <c r="AM75" s="24">
+        <f>70.1666666666667*(-0.303%)+70.1666666666667</f>
+        <v>69.954061666666703</v>
+      </c>
+      <c r="AN75" s="26">
+        <f>1.145*(1-1.34%)</f>
+        <v>1.1296570000000001</v>
+      </c>
+      <c r="AO75" s="23">
+        <f>33.2833333333333*(1-3.8%)</f>
+        <v>32.018566666666636</v>
+      </c>
+      <c r="AP75" s="26">
+        <f>8.96*(1-6.6%)</f>
+        <v>8.368640000000001</v>
+      </c>
+      <c r="AQ75" s="24">
         <v>3.5</v>
       </c>
-      <c r="AR75" s="1">
+      <c r="AR75" s="26">
         <f t="shared" si="26"/>
-        <v>13.851121828475572</v>
-      </c>
-      <c r="AS75" s="1">
+        <v>13.506882948817847</v>
+      </c>
+      <c r="AS75" s="26">
         <f t="shared" si="27"/>
-        <v>10.388341371356679</v>
-      </c>
-      <c r="AT75" s="5">
+        <v>10.130162211613385</v>
+      </c>
+      <c r="AT75" s="23">
         <f t="shared" si="28"/>
-        <v>99.115221294707837</v>
-      </c>
-      <c r="AU75" s="5">
-        <v>1738.3157894736842</v>
-      </c>
-      <c r="AV75" s="4">
+        <v>96.835571204929323</v>
+      </c>
+      <c r="AU75" s="23">
+        <f>1738.31578947368*(1-2.3%)</f>
+        <v>1698.3345263157853</v>
+      </c>
+      <c r="AV75" s="24">
         <v>1918.0526315789473</v>
       </c>
-      <c r="AW75" s="4">
+      <c r="AW75" s="24">
         <v>66.21052631578948</v>
       </c>
-      <c r="AX75" s="1">
-        <v>1.1063157894736844</v>
-      </c>
-      <c r="AY75" s="4">
+      <c r="AX75" s="26">
+        <f>1.10631578947368*(1+2.79%)</f>
+        <v>1.1371819999999957</v>
+      </c>
+      <c r="AY75" s="24">
         <v>29.994736842105269</v>
       </c>
-      <c r="AZ75" s="4">
+      <c r="AZ75" s="24">
         <f t="shared" si="30"/>
-        <v>99.056603773584911</v>
-      </c>
-      <c r="BA75" s="4">
-        <v>157.5</v>
-      </c>
-      <c r="BB75" s="11">
+        <v>96.902981586172558</v>
+      </c>
+      <c r="BA75" s="24">
+        <f>157.5*(1-3.26%)</f>
+        <v>152.3655</v>
+      </c>
+      <c r="BB75" s="27">
         <v>123884.22</v>
       </c>
-      <c r="BC75" s="11">
-        <v>54932.041879999997</v>
-      </c>
-      <c r="BD75" s="11">
-        <v>66285.17254</v>
-      </c>
-      <c r="BE75" s="11">
+      <c r="BC75" s="27">
+        <f>54932.04188*(1+0.15%)</f>
+        <v>55014.439942819998</v>
+      </c>
+      <c r="BD75" s="27">
+        <f>66285.17254*(1-0.163%)</f>
+        <v>66177.127708759799</v>
+      </c>
+      <c r="BE75" s="27">
         <v>39515.747750000002</v>
       </c>
-      <c r="BG75" s="14">
+      <c r="BG75" s="32">
         <v>2793.6388139999999</v>
       </c>
-      <c r="BH75" s="12">
+      <c r="BH75" s="28">
         <v>2961.2571429999998</v>
       </c>
-      <c r="BI75" s="12">
+      <c r="BI75" s="28">
         <v>2823.6868690000001</v>
       </c>
-      <c r="BJ75" s="12">
+      <c r="BJ75" s="28">
         <v>2993.1080809999999</v>
       </c>
-      <c r="BK75" s="4">
+      <c r="BK75" s="24">
         <f t="shared" si="33"/>
         <v>2808.6628415</v>
       </c>
-      <c r="BL75" s="10">
+      <c r="BL75" s="29">
         <f t="shared" si="34"/>
         <v>2977.1826119999996</v>
       </c>
-      <c r="BM75" s="4">
+      <c r="BM75" s="24">
         <v>5</v>
       </c>
-      <c r="BN75" s="1">
+      <c r="BN75" s="26">
         <v>2.06</v>
       </c>
-      <c r="BO75" s="4">
+      <c r="BO75" s="24">
         <v>1</v>
       </c>
-      <c r="BP75" s="4">
+      <c r="BP75" s="24">
         <v>3.6</v>
       </c>
-      <c r="BQ75">
+      <c r="BQ75" s="22">
         <v>104</v>
       </c>
-      <c r="BR75">
+      <c r="BR75" s="22">
         <v>46</v>
       </c>
-      <c r="BS75">
+      <c r="BS75" s="22">
         <v>20</v>
       </c>
-      <c r="BT75">
+      <c r="BT75" s="22">
         <v>43</v>
       </c>
-      <c r="BU75">
+      <c r="BU75" s="22">
         <v>32</v>
       </c>
-      <c r="BV75" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BW75" s="7">
-        <v>150</v>
-      </c>
-      <c r="BX75" s="7">
+      <c r="BV75" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="BW75" s="25">
+        <f>150*(1+0.93%)</f>
+        <v>151.39500000000001</v>
+      </c>
+      <c r="BX75" s="25">
         <v>275</v>
       </c>
-      <c r="BY75">
-        <v>253</v>
-      </c>
-      <c r="BZ75">
-        <v>1339</v>
-      </c>
-      <c r="CA75">
-        <v>258</v>
-      </c>
-      <c r="CB75">
-        <v>1426</v>
+      <c r="BY75" s="22">
+        <f>253*(1-4.38%)</f>
+        <v>241.91860000000003</v>
+      </c>
+      <c r="BZ75" s="22">
+        <f>1339*(1+6.82%)</f>
+        <v>1430.3198</v>
+      </c>
+      <c r="CA75" s="22">
+        <f>258*(1-4.94%)</f>
+        <v>245.25479999999999</v>
+      </c>
+      <c r="CB75" s="22">
+        <f>1426*(1+7.13%)</f>
+        <v>1527.6737999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
+    <row r="76" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="22">
         <v>1</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="23">
         <v>56</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="24">
         <v>26.5</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="22">
         <v>118</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="22">
         <v>75</v>
       </c>
-      <c r="I76">
+      <c r="I76" s="22">
         <v>110</v>
       </c>
-      <c r="J76">
+      <c r="J76" s="22">
         <v>74</v>
       </c>
-      <c r="K76" s="5">
+      <c r="K76" s="23">
         <f t="shared" si="22"/>
         <v>114</v>
       </c>
-      <c r="L76" s="5">
+      <c r="L76" s="23">
         <f t="shared" si="23"/>
         <v>74.5</v>
       </c>
-      <c r="M76" s="4">
+      <c r="M76" s="24">
         <v>174.4</v>
       </c>
-      <c r="N76" s="4">
-        <v>82.4</v>
-      </c>
-      <c r="O76" s="4">
+      <c r="N76" s="24">
+        <f>82.4*(1+0.19%)</f>
+        <v>82.556560000000005</v>
+      </c>
+      <c r="O76" s="24">
         <v>90.5</v>
       </c>
-      <c r="P76" s="4">
+      <c r="P76" s="24">
         <v>90.6</v>
       </c>
-      <c r="Q76" s="4">
+      <c r="Q76" s="24">
         <f t="shared" si="20"/>
         <v>90.55</v>
       </c>
-      <c r="R76" s="5">
+      <c r="R76" s="23">
         <v>25</v>
       </c>
-      <c r="S76">
+      <c r="S76" s="22">
         <v>18.8</v>
       </c>
-      <c r="T76" s="7" t="s">
+      <c r="T76" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="U76" s="4">
+      <c r="U76" s="24">
         <v>-14.7</v>
       </c>
-      <c r="V76" s="4">
+      <c r="V76" s="24">
         <v>-18</v>
       </c>
-      <c r="W76" s="4">
+      <c r="W76" s="24">
         <v>3.4</v>
       </c>
-      <c r="X76" s="4">
+      <c r="X76" s="24">
         <v>-21</v>
       </c>
-      <c r="Y76" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z76" s="4">
+      <c r="Y76" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z76" s="24">
         <v>2028</v>
       </c>
-      <c r="AA76" s="4">
+      <c r="AA76" s="24">
         <v>2049.3333333333335</v>
       </c>
-      <c r="AB76" s="4">
-        <v>2080.5</v>
-      </c>
-      <c r="AC76" s="4">
+      <c r="AB76" s="24">
+        <f>2080.5*(1+2.5%)</f>
+        <v>2132.5124999999998</v>
+      </c>
+      <c r="AC76" s="24">
         <f t="shared" si="24"/>
-        <v>24.61165048543689</v>
-      </c>
-      <c r="AD76" s="4">
+        <v>24.564977029081636</v>
+      </c>
+      <c r="AD76" s="24">
         <f t="shared" si="21"/>
-        <v>24.870550161812297</v>
-      </c>
-      <c r="AE76" s="4">
+        <v>24.823385728927335</v>
+      </c>
+      <c r="AE76" s="24">
         <f t="shared" si="29"/>
-        <v>25.248786407766989</v>
-      </c>
-      <c r="AF76" s="4">
+        <v>25.830927306079609</v>
+      </c>
+      <c r="AF76" s="24">
         <f t="shared" si="25"/>
-        <v>12.095930232558139</v>
-      </c>
-      <c r="AG76" s="5">
-        <f>10.5*60+5</f>
-        <v>635</v>
-      </c>
-      <c r="AH76">
+        <v>12.537494679312459</v>
+      </c>
+      <c r="AG76" s="23">
+        <f>10.5*60+5*(1+0.81%)</f>
+        <v>635.04049999999995</v>
+      </c>
+      <c r="AH76" s="22">
         <v>3.8</v>
       </c>
-      <c r="AI76">
+      <c r="AI76" s="22">
         <v>18</v>
       </c>
-      <c r="AJ76">
+      <c r="AJ76" s="22">
         <v>17</v>
       </c>
-      <c r="AK76">
-        <v>172</v>
-      </c>
-      <c r="AL76" s="5">
+      <c r="AK76" s="22">
+        <f>172*(1-1.11%)</f>
+        <v>170.0908</v>
+      </c>
+      <c r="AL76" s="23">
         <v>2077.8333333333335</v>
       </c>
-      <c r="AM76" s="4">
-        <v>69.833333333333329</v>
-      </c>
-      <c r="AN76" s="1">
-        <v>1.1050000000000002</v>
-      </c>
-      <c r="AO76" s="5">
-        <v>34.249999999999993</v>
-      </c>
-      <c r="AP76" s="1">
-        <v>6.92</v>
-      </c>
-      <c r="AQ76" s="4">
+      <c r="AM76" s="24">
+        <f>69.8333333333333*(-0.303%)+69.8333333333333</f>
+        <v>69.621738333333298</v>
+      </c>
+      <c r="AN76" s="26">
+        <f>1.105*(1-1.34%)</f>
+        <v>1.090193</v>
+      </c>
+      <c r="AO76" s="23">
+        <f>34.25*(1-3.8%)</f>
+        <v>32.948499999999996</v>
+      </c>
+      <c r="AP76" s="26">
+        <f>6.92*(1-6.6%)</f>
+        <v>6.4632799999999992</v>
+      </c>
+      <c r="AQ76" s="24">
         <v>3</v>
       </c>
-      <c r="AR76" s="1">
+      <c r="AR76" s="26">
         <f t="shared" si="26"/>
-        <v>13.089320388349513</v>
-      </c>
-      <c r="AS76" s="1">
+        <v>12.764014392072536</v>
+      </c>
+      <c r="AS76" s="26">
         <f t="shared" si="27"/>
-        <v>9.816990291262135</v>
-      </c>
-      <c r="AT76" s="5">
+        <v>9.5730107940544009</v>
+      </c>
+      <c r="AT76" s="23">
         <f t="shared" si="28"/>
-        <v>52.629798308392971</v>
-      </c>
-      <c r="AU76" s="5">
-        <v>1078.56</v>
-      </c>
-      <c r="AV76" s="4">
+        <v>51.419312947299922</v>
+      </c>
+      <c r="AU76" s="23">
+        <f>1078.56*(1-2.3%)</f>
+        <v>1053.7531199999999</v>
+      </c>
+      <c r="AV76" s="24">
         <v>902.64</v>
       </c>
-      <c r="AW76" s="4">
+      <c r="AW76" s="24">
         <v>32.64</v>
       </c>
-      <c r="AX76" s="1">
-        <v>0.8368000000000001</v>
-      </c>
-      <c r="AY76" s="4">
+      <c r="AX76" s="26">
+        <f>0.8368*(1+2.79%)</f>
+        <v>0.86014672000000003</v>
+      </c>
+      <c r="AY76" s="24">
         <v>21.588000000000001</v>
       </c>
-      <c r="AZ76" s="4">
+      <c r="AZ76" s="24">
         <f t="shared" si="30"/>
-        <v>65.813953488372093</v>
-      </c>
-      <c r="BA76" s="4">
-        <v>113.2</v>
-      </c>
-      <c r="BB76" s="11">
+        <v>64.383070689302428</v>
+      </c>
+      <c r="BA76" s="24">
+        <f>113.2*(1-3.26%)</f>
+        <v>109.50968</v>
+      </c>
+      <c r="BB76" s="27">
         <v>81656.970499999996</v>
       </c>
-      <c r="BC76" s="11">
-        <v>42701.58</v>
-      </c>
-      <c r="BD76" s="11">
-        <v>36622.86</v>
-      </c>
-      <c r="BE76" s="11">
+      <c r="BC76" s="27">
+        <f>42701.58*(1+0.15%)</f>
+        <v>42765.632370000007</v>
+      </c>
+      <c r="BD76" s="27">
+        <f>36622.86*(1-0.163%)</f>
+        <v>36563.164738200001</v>
+      </c>
+      <c r="BE76" s="27">
         <v>19029.759999999998</v>
       </c>
-      <c r="BG76" s="12">
+      <c r="BG76" s="28">
         <v>1289.6793729999999</v>
       </c>
-      <c r="BH76" s="12">
+      <c r="BH76" s="28">
         <v>1367.0601360000001</v>
       </c>
-      <c r="BI76" s="12">
+      <c r="BI76" s="28">
         <v>1316.524026</v>
       </c>
-      <c r="BJ76" s="12">
+      <c r="BJ76" s="28">
         <v>1395.5154669999999</v>
       </c>
-      <c r="BK76" s="4">
+      <c r="BK76" s="24">
         <f t="shared" si="33"/>
         <v>1303.1016995</v>
       </c>
-      <c r="BL76" s="10">
+      <c r="BL76" s="29">
         <f t="shared" si="34"/>
         <v>1381.2878015000001</v>
       </c>
-      <c r="BM76" s="4">
+      <c r="BM76" s="24">
         <v>4.8</v>
       </c>
-      <c r="BN76" s="1">
+      <c r="BN76" s="26">
         <v>2.95</v>
       </c>
-      <c r="BO76" s="1">
+      <c r="BO76" s="26">
         <v>1.2</v>
       </c>
-      <c r="BP76" s="1">
+      <c r="BP76" s="26">
         <v>5</v>
       </c>
-      <c r="BQ76">
+      <c r="BQ76" s="22">
         <v>100</v>
       </c>
-      <c r="BR76">
+      <c r="BR76" s="22">
         <v>23</v>
       </c>
-      <c r="BS76">
+      <c r="BS76" s="22">
         <v>8</v>
       </c>
-      <c r="BT76">
+      <c r="BT76" s="22">
         <v>33</v>
       </c>
-      <c r="BU76">
+      <c r="BU76" s="22">
         <v>40</v>
       </c>
-      <c r="BV76" s="4">
+      <c r="BV76" s="24">
         <v>7.4</v>
       </c>
-      <c r="BW76">
-        <v>170</v>
-      </c>
-      <c r="BX76">
+      <c r="BW76" s="22">
+        <f>170*(1+0.93%)</f>
+        <v>171.58100000000002</v>
+      </c>
+      <c r="BX76" s="22">
         <v>789</v>
       </c>
-      <c r="BY76">
-        <v>330</v>
-      </c>
-      <c r="BZ76">
-        <v>909</v>
-      </c>
-      <c r="CA76">
-        <v>358</v>
-      </c>
-      <c r="CB76">
-        <v>949</v>
+      <c r="BY76" s="22">
+        <f>330*(1-4.38%)</f>
+        <v>315.54599999999999</v>
+      </c>
+      <c r="BZ76" s="22">
+        <f>909*(1+6.82%)</f>
+        <v>970.99380000000008</v>
+      </c>
+      <c r="CA76" s="22">
+        <f>358*(1-4.94%)</f>
+        <v>340.31479999999999</v>
+      </c>
+      <c r="CB76" s="22">
+        <f>949*(1+7.13%)</f>
+        <v>1016.6636999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="8" t="s">
+    <row r="77" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="22">
         <v>1</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="23">
         <v>46</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="24">
         <v>24.7</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="22">
         <v>142</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="22">
         <v>89</v>
       </c>
-      <c r="I77">
+      <c r="I77" s="22">
         <v>139</v>
       </c>
-      <c r="J77">
+      <c r="J77" s="22">
         <v>100</v>
       </c>
-      <c r="K77" s="5">
+      <c r="K77" s="23">
         <f t="shared" si="22"/>
         <v>140.5</v>
       </c>
-      <c r="L77" s="5">
+      <c r="L77" s="23">
         <f t="shared" si="23"/>
         <v>94.5</v>
       </c>
-      <c r="M77" s="4">
+      <c r="M77" s="24">
         <v>166</v>
       </c>
-      <c r="N77" s="4">
-        <v>68.2</v>
-      </c>
-      <c r="O77" s="4">
+      <c r="N77" s="24">
+        <f>68.2*(1+0.19%)</f>
+        <v>68.329580000000007</v>
+      </c>
+      <c r="O77" s="24">
         <v>80</v>
       </c>
-      <c r="P77" s="4">
+      <c r="P77" s="24">
         <v>81</v>
       </c>
-      <c r="Q77" s="4">
+      <c r="Q77" s="24">
         <f t="shared" si="20"/>
         <v>80.5</v>
       </c>
-      <c r="R77" s="5">
+      <c r="R77" s="23">
         <v>20</v>
       </c>
-      <c r="S77" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="T77" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="U77" s="4">
+      <c r="S77" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="T77" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="U77" s="24">
         <v>7.5</v>
       </c>
-      <c r="V77" s="4">
+      <c r="V77" s="24">
         <v>7</v>
       </c>
-      <c r="W77" s="4">
+      <c r="W77" s="24">
         <v>2.5</v>
       </c>
-      <c r="X77" s="4">
+      <c r="X77" s="24">
         <v>-8</v>
       </c>
-      <c r="Y77" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z77" s="4">
+      <c r="Y77" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z77" s="24">
         <v>2203</v>
       </c>
-      <c r="AA77" s="4">
+      <c r="AA77" s="24">
         <v>2196.5</v>
       </c>
-      <c r="AB77" s="4">
-        <v>2241.8333333333335</v>
-      </c>
-      <c r="AC77" s="4">
+      <c r="AB77" s="24">
+        <f>2241.83333333333*(1+2.5%)</f>
+        <v>2297.879166666663</v>
+      </c>
+      <c r="AC77" s="24">
         <f t="shared" si="24"/>
-        <v>32.302052785923749</v>
-      </c>
-      <c r="AD77" s="4">
+        <v>32.240795274901437</v>
+      </c>
+      <c r="AD77" s="24">
         <f t="shared" si="21"/>
-        <v>32.206744868035187</v>
-      </c>
-      <c r="AE77" s="4">
+        <v>32.145668098647754</v>
+      </c>
+      <c r="AE77" s="24">
         <f t="shared" si="29"/>
-        <v>32.871456500488762</v>
-      </c>
-      <c r="AF77" s="4">
+        <v>33.629347153409441</v>
+      </c>
+      <c r="AF77" s="24">
         <f t="shared" si="25"/>
-        <v>13.505020080321286</v>
-      </c>
-      <c r="AG77" s="5">
-        <f>11*60+35</f>
-        <v>695</v>
-      </c>
-      <c r="AH77">
+        <v>13.998023644786425</v>
+      </c>
+      <c r="AG77" s="23">
+        <f>11*60+35*(1+0.81%)</f>
+        <v>695.2835</v>
+      </c>
+      <c r="AH77" s="22">
         <v>4.8</v>
       </c>
-      <c r="AI77">
+      <c r="AI77" s="22">
         <v>20</v>
       </c>
-      <c r="AJ77">
+      <c r="AJ77" s="22">
         <v>20</v>
       </c>
-      <c r="AK77">
-        <v>166</v>
-      </c>
-      <c r="AL77" s="5">
+      <c r="AK77" s="22">
+        <f>166*(1-1.11%)</f>
+        <v>164.1574</v>
+      </c>
+      <c r="AL77" s="23">
         <v>2878.5</v>
       </c>
-      <c r="AM77" s="4">
-        <v>88.333333333333329</v>
-      </c>
-      <c r="AN77" s="1">
-        <v>1.3100000000000003</v>
-      </c>
-      <c r="AO77" s="5">
-        <v>36.133333333333333</v>
-      </c>
-      <c r="AP77" s="1">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="AQ77" s="4">
+      <c r="AM77" s="24">
+        <f>88.3333333333333*(-0.303%)+88.3333333333333</f>
+        <v>88.065683333333297</v>
+      </c>
+      <c r="AN77" s="26">
+        <f>1.31*(1-1.34%)</f>
+        <v>1.2924460000000002</v>
+      </c>
+      <c r="AO77" s="23">
+        <f>36.1333333333333*(1-3.8%)</f>
+        <v>34.760266666666631</v>
+      </c>
+      <c r="AP77" s="26">
+        <f>9.2*(1-6.6%)</f>
+        <v>8.5927999999999987</v>
+      </c>
+      <c r="AQ77" s="24">
         <v>3.5</v>
       </c>
-      <c r="AR77" s="1">
+      <c r="AR77" s="26">
         <f t="shared" si="26"/>
-        <v>16.21524926686217</v>
-      </c>
-      <c r="AS77" s="1">
+        <v>15.812255248751711</v>
+      </c>
+      <c r="AS77" s="26">
         <f t="shared" si="27"/>
-        <v>12.161436950146626</v>
-      </c>
-      <c r="AT77" s="5">
+        <v>11.859191436563783</v>
+      </c>
+      <c r="AT77" s="23">
         <f t="shared" si="28"/>
-        <v>50.347370817209203</v>
-      </c>
-      <c r="AU77" s="5">
-        <v>1105.8800000000001</v>
-      </c>
-      <c r="AV77" s="4">
+        <v>49.189381288413387</v>
+      </c>
+      <c r="AU77" s="23">
+        <f>1105.88*(1-2.3%)</f>
+        <v>1080.4447600000001</v>
+      </c>
+      <c r="AV77" s="24">
         <v>936.48</v>
       </c>
-      <c r="AW77" s="4">
+      <c r="AW77" s="24">
         <v>25.92</v>
       </c>
-      <c r="AX77" s="1">
-        <v>0.84760000000000002</v>
-      </c>
-      <c r="AY77" s="4">
+      <c r="AX77" s="26">
+        <f>0.8476*(1+2.79%)</f>
+        <v>0.87124804</v>
+      </c>
+      <c r="AY77" s="24">
         <v>15.956</v>
       </c>
-      <c r="AZ77" s="4">
+      <c r="AZ77" s="24">
         <f t="shared" si="30"/>
-        <v>48.554216867469876</v>
-      </c>
-      <c r="BA77" s="4">
-        <v>80.599999999999994</v>
-      </c>
-      <c r="BB77" s="11">
+        <v>47.498583676398383</v>
+      </c>
+      <c r="BA77" s="24">
+        <f>80.6*(1-3.26%)</f>
+        <v>77.972439999999992</v>
+      </c>
+      <c r="BB77" s="27">
         <v>67825.422699999996</v>
       </c>
-      <c r="BC77" s="11">
-        <v>39237.406490000001</v>
-      </c>
-      <c r="BD77" s="11">
-        <v>26185.67812</v>
-      </c>
-      <c r="BE77" s="11">
+      <c r="BC77" s="27">
+        <f>39237.40649*(1+0.15%)</f>
+        <v>39296.262599735004</v>
+      </c>
+      <c r="BD77" s="27">
+        <f>26185.67812*(1-0.163%)</f>
+        <v>26142.9954646644</v>
+      </c>
+      <c r="BE77" s="27">
         <v>13984.327670000001</v>
       </c>
-      <c r="BG77" s="12">
+      <c r="BG77" s="28">
         <v>739.48006969999994</v>
       </c>
-      <c r="BH77" s="12">
+      <c r="BH77" s="28">
         <v>783.84887389999994</v>
       </c>
-      <c r="BI77" s="12">
+      <c r="BI77" s="28">
         <v>807.63366589999998</v>
       </c>
-      <c r="BJ77" s="12">
+      <c r="BJ77" s="28">
         <v>856.09168580000005</v>
       </c>
-      <c r="BK77" s="4">
+      <c r="BK77" s="24">
         <f t="shared" si="33"/>
         <v>773.55686779999996</v>
       </c>
-      <c r="BL77" s="10">
+      <c r="BL77" s="29">
         <f t="shared" si="34"/>
         <v>819.97027985</v>
       </c>
-      <c r="BM77" s="4">
+      <c r="BM77" s="24">
         <v>4.5999999999999996</v>
       </c>
-      <c r="BN77" s="1">
+      <c r="BN77" s="26">
         <v>1.53</v>
       </c>
-      <c r="BO77" s="4">
+      <c r="BO77" s="24">
         <v>1.5</v>
       </c>
-      <c r="BP77" s="4">
+      <c r="BP77" s="24">
         <v>3.5</v>
       </c>
-      <c r="BQ77">
+      <c r="BQ77" s="22">
         <v>101</v>
       </c>
-      <c r="BR77">
+      <c r="BR77" s="22">
         <v>35</v>
       </c>
-      <c r="BS77">
+      <c r="BS77" s="22">
         <v>15</v>
       </c>
-      <c r="BT77">
+      <c r="BT77" s="22">
         <v>44</v>
       </c>
-      <c r="BU77">
+      <c r="BU77" s="22">
         <v>30</v>
       </c>
-      <c r="BV77" s="4">
+      <c r="BV77" s="24">
         <v>5.4</v>
       </c>
-      <c r="BW77">
-        <v>190</v>
-      </c>
-      <c r="BX77">
+      <c r="BW77" s="22">
+        <f>190*(1+0.93%)</f>
+        <v>191.76700000000002</v>
+      </c>
+      <c r="BX77" s="22">
         <v>304</v>
       </c>
-      <c r="BY77">
-        <v>168</v>
-      </c>
-      <c r="BZ77">
-        <v>953</v>
-      </c>
-      <c r="CA77">
-        <v>171</v>
-      </c>
-      <c r="CB77">
-        <v>1043</v>
+      <c r="BY77" s="22">
+        <f>168*(1-4.38%)</f>
+        <v>160.64160000000001</v>
+      </c>
+      <c r="BZ77" s="22">
+        <f>953*(1+6.82%)</f>
+        <v>1017.9946</v>
+      </c>
+      <c r="CA77" s="22">
+        <f>171*(1-4.94%)</f>
+        <v>162.55260000000001</v>
+      </c>
+      <c r="CB77" s="22">
+        <f>1043*(1+7.13%)</f>
+        <v>1117.3659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fikset ancova til vo2resualter
</commit_message>
<xml_diff>
--- a/data/Revidert_resultatskjema.xlsx
+++ b/data/Revidert_resultatskjema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3890" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC3697FF-2662-4DED-B773-5B68D158ED6C}"/>
+  <xr:revisionPtr revIDLastSave="3892" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6B761A3-37D2-4CC0-A7CF-5517542287AF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>vo2max_ml_min_kg_6x5</t>
   </si>
   <si>
-    <t>o2_puls (ml)</t>
-  </si>
-  <si>
     <t>time_to_exhaustion</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>CO2_max (ml/min)_30sek</t>
   </si>
   <si>
-    <t>Ve_L/min_max_30sek</t>
-  </si>
-  <si>
     <t>rer_max_30sek</t>
   </si>
   <si>
@@ -740,6 +734,12 @@
   </si>
   <si>
     <t>one_rm_watt</t>
+  </si>
+  <si>
+    <t>o2_puls_ml</t>
+  </si>
+  <si>
+    <t>Ve_L_min_max_30sek</t>
   </si>
 </sst>
 </file>
@@ -1193,9 +1193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BX73" sqref="BX73"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1408,447 +1408,447 @@
         <v>30</v>
       </c>
       <c r="AF1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AS1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AT1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="19" t="s">
+      <c r="AU1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="19" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="20" t="s">
+      <c r="AW1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="19" t="s">
+      <c r="AY1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BL1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BM1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BT1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
+        <v>231</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>232</v>
+      </c>
+      <c r="BY1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BZ1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
-        <v>233</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>234</v>
-      </c>
-      <c r="BY1" t="s">
+      <c r="CA1" t="s">
         <v>74</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CB1" t="s">
         <v>75</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
         <v>76</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CD1" t="s">
         <v>77</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CE1" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CF1" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CG1" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CH1" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CI1" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CJ1" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CK1" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CL1" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CM1" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CN1" t="s">
         <v>87</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CO1" t="s">
         <v>88</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CP1" t="s">
         <v>89</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CQ1" t="s">
         <v>90</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CR1" t="s">
         <v>91</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CS1" t="s">
         <v>92</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CT1" t="s">
         <v>93</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CU1" t="s">
         <v>94</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CV1" t="s">
         <v>95</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CW1" t="s">
         <v>96</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CX1" t="s">
         <v>97</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CY1" t="s">
         <v>98</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CZ1" t="s">
         <v>99</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DA1" t="s">
         <v>100</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DB1" t="s">
         <v>101</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DC1" t="s">
         <v>102</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DD1" t="s">
         <v>103</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DE1" t="s">
         <v>104</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DF1" t="s">
         <v>105</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DG1" t="s">
         <v>106</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DH1" t="s">
         <v>107</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DI1" t="s">
         <v>108</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DJ1" t="s">
         <v>109</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DK1" t="s">
         <v>110</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DL1" t="s">
         <v>111</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DM1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DN1" t="s">
         <v>113</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DO1" t="s">
         <v>114</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DP1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DQ1" t="s">
         <v>116</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DR1" t="s">
         <v>117</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DS1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DT1" t="s">
         <v>119</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DU1" t="s">
         <v>120</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DV1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DW1" t="s">
         <v>122</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="DX1" t="s">
         <v>123</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DY1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DZ1" t="s">
         <v>125</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EA1" t="s">
         <v>126</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EB1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EC1" t="s">
         <v>128</v>
       </c>
-      <c r="EB1" s="2" t="s">
+      <c r="ED1" t="s">
         <v>129</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="EE1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EF1" t="s">
         <v>131</v>
       </c>
-      <c r="EE1" s="2" t="s">
+      <c r="EG1" t="s">
         <v>132</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EH1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EI1" t="s">
         <v>134</v>
       </c>
-      <c r="EH1" s="2" t="s">
+      <c r="EJ1" t="s">
         <v>135</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EK1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EL1" t="s">
         <v>137</v>
       </c>
-      <c r="EK1" s="2" t="s">
+      <c r="EM1" t="s">
         <v>138</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EN1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EO1" t="s">
         <v>140</v>
       </c>
-      <c r="EN1" s="2" t="s">
+      <c r="EP1" t="s">
         <v>141</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EQ1" t="s">
         <v>142</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="ER1" t="s">
         <v>143</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ES1" t="s">
         <v>144</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ET1" t="s">
         <v>145</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="EU1" t="s">
         <v>146</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EV1" t="s">
         <v>147</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EW1" t="s">
         <v>148</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EX1" t="s">
         <v>149</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EY1" t="s">
         <v>150</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EZ1" t="s">
         <v>151</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FA1" t="s">
         <v>152</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FB1" t="s">
         <v>153</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FC1" t="s">
         <v>154</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FD1" t="s">
         <v>155</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FE1" t="s">
         <v>156</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="FF1" t="s">
         <v>157</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="FG1" t="s">
         <v>158</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="FH1" t="s">
         <v>159</v>
       </c>
-      <c r="FG1" t="s">
+      <c r="FI1" t="s">
         <v>160</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FJ1" t="s">
         <v>161</v>
       </c>
-      <c r="FI1" t="s">
+      <c r="FK1" t="s">
         <v>162</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="FL1" t="s">
         <v>163</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FM1" t="s">
         <v>164</v>
       </c>
-      <c r="FL1" t="s">
+      <c r="FN1" t="s">
         <v>165</v>
       </c>
-      <c r="FM1" t="s">
+      <c r="FO1" t="s">
         <v>166</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="FP1" t="s">
         <v>167</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="FQ1" t="s">
         <v>168</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="FR1" t="s">
         <v>169</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="FS1" t="s">
         <v>170</v>
-      </c>
-      <c r="FR1" t="s">
-        <v>171</v>
-      </c>
-      <c r="FS1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" t="s">
-        <v>175</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1902,7 +1902,7 @@
         <v>74</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U2" s="4">
         <v>20</v>
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z2" s="4">
         <v>2587</v>
@@ -2095,13 +2095,13 @@
     </row>
     <row r="3" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2155,7 +2155,7 @@
         <v>42.8</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U3" s="4">
         <v>-14</v>
@@ -2170,7 +2170,7 @@
         <v>-10.4</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z3" s="4">
         <v>2937.5</v>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="4" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2408,7 +2408,7 @@
         <v>13.5</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U4" s="4">
         <v>-7.5</v>
@@ -2583,7 +2583,7 @@
         <v>190</v>
       </c>
       <c r="BX4" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY4">
         <v>172</v>
@@ -2600,13 +2600,13 @@
     </row>
     <row r="5" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2660,7 +2660,7 @@
         <v>5.8</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U5" s="4">
         <v>3</v>
@@ -2675,7 +2675,7 @@
         <v>-34</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z5" s="4">
         <v>2004</v>
@@ -2853,13 +2853,13 @@
     </row>
     <row r="6" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2913,7 +2913,7 @@
         <v>73.5</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U6" s="4">
         <v>12.5</v>
@@ -2928,7 +2928,7 @@
         <v>5.5</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z6" s="4">
         <v>3131</v>
@@ -3098,21 +3098,21 @@
         <v>552</v>
       </c>
       <c r="CA6" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB6" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3166,7 +3166,7 @@
         <v>66</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U7" s="4">
         <v>7.5</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="8" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -3419,7 +3419,7 @@
         <v>64</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U8" s="4">
         <v>-12.5</v>
@@ -3434,7 +3434,7 @@
         <v>-3</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z8" s="4">
         <v>3715</v>
@@ -3612,13 +3612,13 @@
     </row>
     <row r="9" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3672,7 +3672,7 @@
         <v>64</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U9" s="4">
         <v>16</v>
@@ -3687,7 +3687,7 @@
         <v>6</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z9" s="4">
         <v>1623</v>
@@ -3842,7 +3842,7 @@
         <v>45</v>
       </c>
       <c r="BV9" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW9" s="7">
         <v>135</v>
@@ -3865,13 +3865,13 @@
     </row>
     <row r="10" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3925,7 +3925,7 @@
         <v>48.6</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U10" s="4">
         <v>2</v>
@@ -3940,7 +3940,7 @@
         <v>-20</v>
       </c>
       <c r="Y10" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z10" s="4">
         <v>2328.5</v>
@@ -4118,13 +4118,13 @@
     </row>
     <row r="11" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -4178,7 +4178,7 @@
         <v>65</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U11" s="4">
         <v>7</v>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="Y11" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z11" s="4">
         <v>1711</v>
@@ -4354,7 +4354,7 @@
         <v>180</v>
       </c>
       <c r="BX11" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY11">
         <v>292</v>
@@ -4371,13 +4371,13 @@
     </row>
     <row r="12" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -4431,7 +4431,7 @@
         <v>51.7</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U12" s="4">
         <v>-0.2</v>
@@ -4624,13 +4624,13 @@
     </row>
     <row r="13" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -4684,7 +4684,7 @@
         <v>66.3</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U13" s="4">
         <v>12.1</v>
@@ -4699,7 +4699,7 @@
         <v>2.5</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z13" s="4">
         <v>2589.5</v>
@@ -4877,13 +4877,13 @@
     </row>
     <row r="14" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -4937,7 +4937,7 @@
         <v>43.4</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U14" s="4">
         <v>0</v>
@@ -4952,7 +4952,7 @@
         <v>-8.5</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z14" s="4">
         <v>2579</v>
@@ -5106,7 +5106,7 @@
         <v>33</v>
       </c>
       <c r="BV14" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW14" s="7">
         <v>320</v>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="15" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -5189,7 +5189,7 @@
         <v>11</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U15" s="4">
         <v>3</v>
@@ -5382,13 +5382,13 @@
     </row>
     <row r="16" spans="1:175" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -5442,7 +5442,7 @@
         <v>12.8</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U16" s="4">
         <v>-12</v>
@@ -5457,7 +5457,7 @@
         <v>-7.3</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z16" s="4">
         <v>3146</v>
@@ -5585,16 +5585,16 @@
         <v>3459.6962569999996</v>
       </c>
       <c r="BM16" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN16" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO16" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP16" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ16">
         <v>142</v>
@@ -5635,13 +5635,13 @@
     </row>
     <row r="17" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -5695,7 +5695,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U17" s="4">
         <v>-19.8</v>
@@ -5710,7 +5710,7 @@
         <v>-15.2</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z17" s="4">
         <v>2581.5</v>
@@ -5871,7 +5871,7 @@
         <v>195</v>
       </c>
       <c r="BX17" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY17">
         <v>428</v>
@@ -5888,13 +5888,13 @@
     </row>
     <row r="18" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -5948,7 +5948,7 @@
         <v>69</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U18" s="4">
         <v>6.5</v>
@@ -5963,7 +5963,7 @@
         <v>-4</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z18" s="4">
         <v>2592</v>
@@ -6071,22 +6071,22 @@
         <v>6245.3818069999998</v>
       </c>
       <c r="BG18" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BH18" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BI18" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BJ18" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BK18" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BL18" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BM18" s="4">
         <v>5.0999999999999996</v>
@@ -6139,13 +6139,13 @@
     </row>
     <row r="19" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -6199,7 +6199,7 @@
         <v>31.6</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U19" s="4">
         <v>5.2</v>
@@ -6214,7 +6214,7 @@
         <v>-29.7</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z19" s="4">
         <v>1744</v>
@@ -6369,7 +6369,7 @@
         <v>32</v>
       </c>
       <c r="BV19" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW19" s="7">
         <v>150</v>
@@ -6392,13 +6392,13 @@
     </row>
     <row r="20" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -6452,7 +6452,7 @@
         <v>4.2</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U20">
         <v>7.2</v>
@@ -6461,7 +6461,7 @@
         <v>8</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="X20" s="4">
         <v>-26</v>
@@ -6595,16 +6595,16 @@
         <v>3382.5972730000003</v>
       </c>
       <c r="BM20" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN20" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO20" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP20" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ20">
         <v>121</v>
@@ -6645,13 +6645,13 @@
     </row>
     <row r="21" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -6705,7 +6705,7 @@
         <v>3.3</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U21" s="4">
         <v>2.2000000000000002</v>
@@ -6720,7 +6720,7 @@
         <v>-5</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z21" s="4">
         <v>2167.5</v>
@@ -6898,13 +6898,13 @@
     </row>
     <row r="22" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -6958,7 +6958,7 @@
         <v>5.7</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U22" s="4">
         <v>-17.5</v>
@@ -6973,7 +6973,7 @@
         <v>-60</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z22" s="4">
         <v>2703.5</v>
@@ -7151,13 +7151,13 @@
     </row>
     <row r="23" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -7211,7 +7211,7 @@
         <v>87.3</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U23" s="4">
         <v>27.3</v>
@@ -7226,7 +7226,7 @@
         <v>15</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z23" s="4">
         <v>4555</v>
@@ -7404,13 +7404,13 @@
     </row>
     <row r="24" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -7464,7 +7464,7 @@
         <v>18.8</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U24" s="4">
         <v>-14.7</v>
@@ -7479,7 +7479,7 @@
         <v>-21</v>
       </c>
       <c r="Y24" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z24" s="4">
         <v>2028</v>
@@ -7657,13 +7657,13 @@
     </row>
     <row r="25" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -7717,7 +7717,7 @@
         <v>52.5</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U25">
         <v>1.8</v>
@@ -7732,7 +7732,7 @@
         <v>-9.5</v>
       </c>
       <c r="Y25" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z25" s="4">
         <v>2871.5</v>
@@ -7910,13 +7910,13 @@
     </row>
     <row r="26" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -7970,7 +7970,7 @@
         <v>65</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U26" s="4">
         <v>8</v>
@@ -7985,7 +7985,7 @@
         <v>3.5</v>
       </c>
       <c r="Y26" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z26" s="4">
         <v>2983</v>
@@ -8009,7 +8009,7 @@
         <v>38.480881130507065</v>
       </c>
       <c r="AF26" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AG26" s="5">
         <f>14*60+5</f>
@@ -8025,7 +8025,7 @@
         <v>20</v>
       </c>
       <c r="AK26" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AL26" s="5">
         <v>4053</v>
@@ -8073,10 +8073,10 @@
         <v>22.772000000000002</v>
       </c>
       <c r="AZ26" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BA26" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BB26" s="11">
         <v>79257.789980000001</v>
@@ -8161,13 +8161,13 @@
     </row>
     <row r="27" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -8221,7 +8221,7 @@
         <v>66</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U27" s="4">
         <v>8</v>
@@ -8414,13 +8414,13 @@
     </row>
     <row r="28" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -8474,7 +8474,7 @@
         <v>68.5</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U28" s="4">
         <v>-3</v>
@@ -8489,7 +8489,7 @@
         <v>1</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z28" s="4">
         <v>3234</v>
@@ -8667,13 +8667,13 @@
     </row>
     <row r="29" spans="1:80" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -8727,7 +8727,7 @@
         <v>73.7</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U29" s="4">
         <v>17.3</v>
@@ -8742,7 +8742,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z29" s="4">
         <v>2729</v>
@@ -8850,22 +8850,22 @@
         <v>16707.703570000001</v>
       </c>
       <c r="BG29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BH29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BI29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BJ29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BK29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BL29" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BM29" s="4">
         <v>4.2</v>
@@ -8918,13 +8918,13 @@
     </row>
     <row r="30" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -8978,7 +8978,7 @@
         <v>66.599999999999994</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U30" s="4">
         <v>12.3</v>
@@ -8993,7 +8993,7 @@
         <v>-4.5</v>
       </c>
       <c r="Y30" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z30" s="4">
         <v>3931</v>
@@ -9171,13 +9171,13 @@
     </row>
     <row r="31" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -9231,7 +9231,7 @@
         <v>3.6</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U31" s="4">
         <v>-3.5</v>
@@ -9246,7 +9246,7 @@
         <v>-15</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z31" s="4">
         <v>2062</v>
@@ -9416,21 +9416,21 @@
         <v>1164</v>
       </c>
       <c r="CA31" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB31" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -9484,7 +9484,7 @@
         <v>47.1</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U32" s="4">
         <v>7</v>
@@ -9499,7 +9499,7 @@
         <v>-8</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z32" s="4">
         <v>1790</v>
@@ -9677,13 +9677,13 @@
     </row>
     <row r="33" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -9737,7 +9737,7 @@
         <v>28.3</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U33" s="4">
         <v>3.2</v>
@@ -9752,7 +9752,7 @@
         <v>-14.4</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z33" s="4">
         <v>2223</v>
@@ -9930,13 +9930,13 @@
     </row>
     <row r="34" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -9990,7 +9990,7 @@
         <v>73.5</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U34" s="4">
         <v>-10.5</v>
@@ -10005,7 +10005,7 @@
         <v>-21.5</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z34" s="4">
         <v>3195</v>
@@ -10183,13 +10183,13 @@
     </row>
     <row r="35" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -10243,7 +10243,7 @@
         <v>6.6</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U35" s="4">
         <v>6.8</v>
@@ -10258,7 +10258,7 @@
         <v>-18</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z35" s="4">
         <v>2304</v>
@@ -10436,13 +10436,13 @@
     </row>
     <row r="36" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -10496,7 +10496,7 @@
         <v>35.5</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U36" s="4">
         <v>3</v>
@@ -10511,7 +10511,7 @@
         <v>-4.5</v>
       </c>
       <c r="Y36" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z36" s="4">
         <v>2544.5</v>
@@ -10689,13 +10689,13 @@
     </row>
     <row r="37" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -10749,7 +10749,7 @@
         <v>70.3</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U37" s="4">
         <v>22</v>
@@ -10764,7 +10764,7 @@
         <v>-11.5</v>
       </c>
       <c r="Y37" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z37" s="4">
         <v>2241.5</v>
@@ -10942,13 +10942,13 @@
     </row>
     <row r="38" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -10999,10 +10999,10 @@
         <v>20</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U38" s="4">
         <v>7.5</v>
@@ -11017,7 +11017,7 @@
         <v>-8</v>
       </c>
       <c r="Y38" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z38" s="4">
         <v>2203</v>
@@ -11195,13 +11195,13 @@
     </row>
     <row r="39" spans="1:80" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -11255,7 +11255,7 @@
         <v>68</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U39" s="4">
         <v>3</v>
@@ -11366,96 +11366,96 @@
         <v>97</v>
       </c>
       <c r="BB39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BC39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BD39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BE39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BF39" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BG39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BH39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BI39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BJ39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BK39" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BL39" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BM39" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN39" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO39" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP39" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BR39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BS39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BT39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BU39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BV39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BX39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BZ39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CA39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -11509,7 +11509,7 @@
         <v>64</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U40" s="4">
         <v>22</v>
@@ -11524,7 +11524,7 @@
         <v>3</v>
       </c>
       <c r="Y40" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z40" s="4">
         <v>2878</v>
@@ -11702,13 +11702,13 @@
     </row>
     <row r="41" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -11762,7 +11762,7 @@
         <v>44.8</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U41" s="4">
         <v>4.8</v>
@@ -11955,13 +11955,13 @@
     </row>
     <row r="42" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -12015,7 +12015,7 @@
         <v>66.400000000000006</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U42" s="4">
         <v>-17</v>
@@ -12030,7 +12030,7 @@
         <v>-12</v>
       </c>
       <c r="Y42" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z42" s="4">
         <v>3171</v>
@@ -12208,13 +12208,13 @@
     </row>
     <row r="43" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -12268,7 +12268,7 @@
         <v>5.2</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U43" s="4">
         <v>-6.5</v>
@@ -12410,16 +12410,16 @@
         <v>2227.4087015</v>
       </c>
       <c r="BM43" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN43" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO43" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP43" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ43">
         <v>128</v>
@@ -12460,13 +12460,13 @@
     </row>
     <row r="44" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -12520,7 +12520,7 @@
         <v>104.9</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U44" s="4">
         <v>15</v>
@@ -12535,7 +12535,7 @@
         <v>0</v>
       </c>
       <c r="Y44" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z44" s="4">
         <v>1746</v>
@@ -12713,13 +12713,13 @@
     </row>
     <row r="45" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -12773,7 +12773,7 @@
         <v>5.7</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U45" s="4">
         <v>-22</v>
@@ -12916,16 +12916,16 @@
         <v>1562.2461375</v>
       </c>
       <c r="BM45" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN45" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO45" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP45" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ45">
         <v>128</v>
@@ -12966,13 +12966,13 @@
     </row>
     <row r="46" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -13026,7 +13026,7 @@
         <v>7</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U46" s="4">
         <v>2</v>
@@ -13219,13 +13219,13 @@
     </row>
     <row r="47" spans="1:80" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -13279,7 +13279,7 @@
         <v>66</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U47" s="4">
         <v>3.5</v>
@@ -13390,96 +13390,96 @@
         <v>105</v>
       </c>
       <c r="BB47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BC47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BD47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BE47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BF47" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BG47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BH47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BI47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BJ47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BK47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BL47" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BM47" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN47" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO47" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP47" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BR47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BS47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BT47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BU47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BV47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BX47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BZ47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CA47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB47" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -13533,7 +13533,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U48" s="4">
         <v>16.2</v>
@@ -13548,7 +13548,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="Y48" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z48" s="4">
         <v>1863</v>
@@ -13726,13 +13726,13 @@
     </row>
     <row r="49" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C49" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -13786,7 +13786,7 @@
         <v>66.599999999999994</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U49" s="4">
         <v>11</v>
@@ -13801,7 +13801,7 @@
         <v>6</v>
       </c>
       <c r="Y49" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z49" s="4">
         <v>3084.5</v>
@@ -13971,21 +13971,21 @@
         <v>583</v>
       </c>
       <c r="CA49" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB49" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -14039,7 +14039,7 @@
         <v>21.75</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U50" s="4">
         <v>-0.5</v>
@@ -14232,13 +14232,13 @@
     </row>
     <row r="51" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C51" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -14292,7 +14292,7 @@
         <v>65</v>
       </c>
       <c r="T51" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U51" s="4">
         <v>14</v>
@@ -14307,7 +14307,7 @@
         <v>1.5</v>
       </c>
       <c r="Y51" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z51" s="4">
         <v>2692</v>
@@ -14485,13 +14485,13 @@
     </row>
     <row r="52" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -14545,7 +14545,7 @@
         <v>48.4</v>
       </c>
       <c r="T52" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U52" s="4">
         <v>8</v>
@@ -14560,7 +14560,7 @@
         <v>-7.6</v>
       </c>
       <c r="Y52" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z52" s="4">
         <v>2675.5</v>
@@ -14714,7 +14714,7 @@
         <v>30</v>
       </c>
       <c r="BV52" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW52">
         <v>311</v>
@@ -14737,13 +14737,13 @@
     </row>
     <row r="53" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -14797,7 +14797,7 @@
         <v>15.8</v>
       </c>
       <c r="T53" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U53" s="4">
         <v>-25</v>
@@ -14812,7 +14812,7 @@
         <v>-5.8</v>
       </c>
       <c r="Y53" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z53" s="4">
         <v>3199.5</v>
@@ -14940,16 +14940,16 @@
         <v>3199.54151</v>
       </c>
       <c r="BM53" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN53" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO53" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP53" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ53">
         <v>132</v>
@@ -14973,7 +14973,7 @@
         <v>300</v>
       </c>
       <c r="BX53" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY53">
         <v>655</v>
@@ -14990,13 +14990,13 @@
     </row>
     <row r="54" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -15050,7 +15050,7 @@
         <v>63</v>
       </c>
       <c r="T54" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U54" s="4">
         <v>0</v>
@@ -15065,7 +15065,7 @@
         <v>-18</v>
       </c>
       <c r="Y54" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z54" s="4">
         <v>2439.5</v>
@@ -15243,13 +15243,13 @@
     </row>
     <row r="55" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -15303,7 +15303,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="T55" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U55" s="4">
         <v>7.5</v>
@@ -15446,16 +15446,16 @@
         <v>3506.4492365000001</v>
       </c>
       <c r="BM55" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN55" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO55" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP55" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ55">
         <v>115</v>
@@ -15496,13 +15496,13 @@
     </row>
     <row r="56" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -15556,7 +15556,7 @@
         <v>64</v>
       </c>
       <c r="T56" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U56" s="4">
         <v>5</v>
@@ -15571,7 +15571,7 @@
         <v>-3</v>
       </c>
       <c r="Y56" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z56" s="4">
         <v>2547.5</v>
@@ -15749,13 +15749,13 @@
     </row>
     <row r="57" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -15809,7 +15809,7 @@
         <v>64.8</v>
       </c>
       <c r="T57" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U57" s="4">
         <v>15.5</v>
@@ -15824,7 +15824,7 @@
         <v>-38</v>
       </c>
       <c r="Y57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z57" s="4">
         <v>2704.5</v>
@@ -15982,33 +15982,33 @@
         <v>7</v>
       </c>
       <c r="BW57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BX57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BY57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BZ57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CA57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="CB57" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -16062,7 +16062,7 @@
         <v>66.3</v>
       </c>
       <c r="T58" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U58" s="4">
         <v>5.6</v>
@@ -16077,7 +16077,7 @@
         <v>-10.199999999999999</v>
       </c>
       <c r="Y58" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z58" s="4">
         <v>2922</v>
@@ -16255,13 +16255,13 @@
     </row>
     <row r="59" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C59" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -16315,7 +16315,7 @@
         <v>20</v>
       </c>
       <c r="T59" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U59" s="4">
         <v>28</v>
@@ -16330,7 +16330,7 @@
         <v>13.5</v>
       </c>
       <c r="Y59" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z59">
         <v>4659.5</v>
@@ -16508,13 +16508,13 @@
     </row>
     <row r="60" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -16568,7 +16568,7 @@
         <v>18.2</v>
       </c>
       <c r="T60" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U60" s="4">
         <v>4.8</v>
@@ -16583,7 +16583,7 @@
         <v>-13.4</v>
       </c>
       <c r="Y60" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z60" s="4">
         <v>3889</v>
@@ -16710,16 +16710,16 @@
         <v>908.44730279999999</v>
       </c>
       <c r="BM60" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BN60" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BO60" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BP60" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BQ60">
         <v>130</v>
@@ -16758,30 +16758,30 @@
         <v>2672</v>
       </c>
       <c r="FT60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="FU60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="FV60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="FW60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="FX60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C61" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -16836,7 +16836,7 @@
         <v>75.06</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U61" s="4">
         <v>-1</v>
@@ -16851,7 +16851,7 @@
         <v>4.5</v>
       </c>
       <c r="Y61" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z61" s="4">
         <v>3573.5</v>
@@ -17029,13 +17029,13 @@
     </row>
     <row r="62" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -17089,7 +17089,7 @@
         <v>63.1</v>
       </c>
       <c r="T62" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U62" s="4">
         <v>10.5</v>
@@ -17104,7 +17104,7 @@
         <v>4</v>
       </c>
       <c r="Y62" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z62" s="4">
         <v>3232</v>
@@ -17282,13 +17282,13 @@
     </row>
     <row r="63" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -17342,7 +17342,7 @@
         <v>24.9</v>
       </c>
       <c r="T63" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U63" s="4">
         <v>3.7</v>
@@ -17357,7 +17357,7 @@
         <v>-19</v>
       </c>
       <c r="Y63" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z63" s="4">
         <v>2382</v>
@@ -17535,13 +17535,13 @@
     </row>
     <row r="64" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -17595,7 +17595,7 @@
         <v>19.5</v>
       </c>
       <c r="T64" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U64" s="4">
         <v>-3.05</v>
@@ -17610,91 +17610,91 @@
         <v>-14</v>
       </c>
       <c r="Y64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AB64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AC64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AD64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE64" s="6">
         <v>21.7254</v>
       </c>
       <c r="AF64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AG64" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AH64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AI64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AJ64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AK64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AL64" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AM64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AN64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AO64" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AP64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AQ64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AR64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AS64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AT64" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AU64" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AV64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AW64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AX64" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AY64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AZ64" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BA64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BB64" s="4">
         <v>97333.78</v>
@@ -17756,7 +17756,7 @@
         <v>34</v>
       </c>
       <c r="BV64" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW64">
         <v>270</v>
@@ -17779,13 +17779,13 @@
     </row>
     <row r="65" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -17839,7 +17839,7 @@
         <v>66</v>
       </c>
       <c r="T65" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U65" s="4">
         <v>7</v>
@@ -17854,7 +17854,7 @@
         <v>-9</v>
       </c>
       <c r="Y65" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z65" s="4">
         <v>1884</v>
@@ -18032,13 +18032,13 @@
     </row>
     <row r="66" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -18092,7 +18092,7 @@
         <v>61.6</v>
       </c>
       <c r="T66" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U66" s="4">
         <v>5</v>
@@ -18107,7 +18107,7 @@
         <v>-5.5</v>
       </c>
       <c r="Y66" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z66" s="4">
         <v>2291</v>
@@ -18285,13 +18285,13 @@
     </row>
     <row r="67" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C67" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -18345,7 +18345,7 @@
         <v>5.34</v>
       </c>
       <c r="T67" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U67" s="4">
         <v>3</v>
@@ -18360,7 +18360,7 @@
         <v>-16.5</v>
       </c>
       <c r="Y67" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z67" s="4">
         <v>1973</v>
@@ -18537,13 +18537,13 @@
     </row>
     <row r="68" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C68" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -18597,7 +18597,7 @@
         <v>64.7</v>
       </c>
       <c r="T68" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U68" s="4">
         <v>-15.5</v>
@@ -18612,7 +18612,7 @@
         <v>-19.3</v>
       </c>
       <c r="Y68" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z68" s="4">
         <v>3058</v>
@@ -18790,13 +18790,13 @@
     </row>
     <row r="69" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C69" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -18850,7 +18850,7 @@
         <v>32</v>
       </c>
       <c r="T69" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U69" s="4">
         <v>6.5</v>
@@ -18865,7 +18865,7 @@
         <v>-5</v>
       </c>
       <c r="Y69" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z69">
         <v>2355.5</v>
@@ -19042,13 +19042,13 @@
     </row>
     <row r="70" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -19103,7 +19103,7 @@
         <v>123.2</v>
       </c>
       <c r="T70" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U70" s="4">
         <v>16.399999999999999</v>
@@ -19118,7 +19118,7 @@
         <v>-7.1</v>
       </c>
       <c r="Y70" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z70" s="4">
         <v>2226</v>
@@ -19296,13 +19296,13 @@
     </row>
     <row r="71" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D71" s="22">
         <v>1</v>
@@ -19357,7 +19357,7 @@
         <v>5.8</v>
       </c>
       <c r="T71" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U71" s="24">
         <v>3</v>
@@ -19372,7 +19372,7 @@
         <v>-34</v>
       </c>
       <c r="Y71" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z71" s="24">
         <v>2004</v>
@@ -19566,13 +19566,13 @@
     </row>
     <row r="72" spans="1:80" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D72" s="22">
         <v>1</v>
@@ -19627,7 +19627,7 @@
         <v>73.7</v>
       </c>
       <c r="T72" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U72" s="24">
         <v>17.3</v>
@@ -19642,7 +19642,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="Y72" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z72" s="24">
         <v>2729</v>
@@ -19761,22 +19761,22 @@
         <v>16707.703570000001</v>
       </c>
       <c r="BG72" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BH72" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BI72" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BJ72" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BK72" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BL72" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BM72" s="24">
         <v>4.2</v>
@@ -19834,13 +19834,13 @@
     </row>
     <row r="73" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D73" s="22">
         <v>1</v>
@@ -19895,7 +19895,7 @@
         <v>66</v>
       </c>
       <c r="T73" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U73" s="24">
         <v>8</v>
@@ -20104,13 +20104,13 @@
     </row>
     <row r="74" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D74" s="22">
         <v>2</v>
@@ -20165,7 +20165,7 @@
         <v>64</v>
       </c>
       <c r="T74" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U74" s="24">
         <v>-12.5</v>
@@ -20180,7 +20180,7 @@
         <v>-3</v>
       </c>
       <c r="Y74" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z74" s="24">
         <v>3715</v>
@@ -20374,13 +20374,13 @@
     </row>
     <row r="75" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D75" s="22">
         <v>1</v>
@@ -20435,7 +20435,7 @@
         <v>31.6</v>
       </c>
       <c r="T75" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U75" s="24">
         <v>5.2</v>
@@ -20450,7 +20450,7 @@
         <v>-29.7</v>
       </c>
       <c r="Y75" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z75" s="24">
         <v>1744</v>
@@ -20616,7 +20616,7 @@
         <v>32</v>
       </c>
       <c r="BV75" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="BW75" s="25">
         <f>150*(1+0.93%)</f>
@@ -20644,13 +20644,13 @@
     </row>
     <row r="76" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D76" s="22">
         <v>1</v>
@@ -20705,7 +20705,7 @@
         <v>18.8</v>
       </c>
       <c r="T76" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U76" s="24">
         <v>-14.7</v>
@@ -20720,7 +20720,7 @@
         <v>-21</v>
       </c>
       <c r="Y76" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z76" s="24">
         <v>2028</v>
@@ -20914,13 +20914,13 @@
     </row>
     <row r="77" spans="1:80" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="22" t="s">
         <v>215</v>
-      </c>
-      <c r="B77" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>217</v>
       </c>
       <c r="D77" s="22">
         <v>1</v>
@@ -20972,10 +20972,10 @@
         <v>20</v>
       </c>
       <c r="S77" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T77" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U77" s="24">
         <v>7.5</v>
@@ -20990,7 +20990,7 @@
         <v>-8</v>
       </c>
       <c r="Y77" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z77" s="24">
         <v>2203</v>
@@ -21200,15 +21200,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -21216,7 +21216,7 @@
         <v>11451</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -21224,7 +21224,7 @@
         <v>15448</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -21232,15 +21232,15 @@
         <v>11442</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -21248,15 +21248,15 @@
         <v>11421</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -21276,47 +21276,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ferdig med p-verider? og ordnet opp i parra t-tester
</commit_message>
<xml_diff>
--- a/data/Revidert_resultatskjema.xlsx
+++ b/data/Revidert_resultatskjema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4002" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C4E3177-37D8-4D80-A9E9-D3086023D135}"/>
+  <xr:revisionPtr revIDLastSave="4061" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6939572F-81A7-42BE-88DE-F5326937568B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="235">
   <si>
     <t>id</t>
   </si>
@@ -817,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -874,6 +874,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,9 +1191,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ26" sqref="AZ26"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CC27" sqref="CC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2579,8 +2580,9 @@
       <c r="BW4" s="7">
         <v>190</v>
       </c>
-      <c r="BX4" s="7" t="s">
-        <v>175</v>
+      <c r="BX4" s="7">
+        <f>290*(1-46%)</f>
+        <v>156.60000000000002</v>
       </c>
       <c r="BY4">
         <v>172</v>
@@ -4350,8 +4352,9 @@
       <c r="BW11" s="7">
         <v>180</v>
       </c>
-      <c r="BX11" s="7" t="s">
-        <v>175</v>
+      <c r="BX11" s="7">
+        <f>289*(1-46%)</f>
+        <v>156.06</v>
       </c>
       <c r="BY11">
         <v>292</v>
@@ -5706,8 +5709,8 @@
       <c r="X17" s="4">
         <v>-15.2</v>
       </c>
-      <c r="Y17" s="7" t="s">
-        <v>175</v>
+      <c r="Y17" s="7">
+        <v>10</v>
       </c>
       <c r="Z17" s="4">
         <v>2581.5</v>
@@ -5867,8 +5870,9 @@
       <c r="BW17" s="7">
         <v>195</v>
       </c>
-      <c r="BX17" s="7" t="s">
-        <v>175</v>
+      <c r="BX17" s="7">
+        <f>574*(1-46%)</f>
+        <v>309.96000000000004</v>
       </c>
       <c r="BY17">
         <v>428</v>
@@ -9415,11 +9419,13 @@
       <c r="BZ31">
         <v>1164</v>
       </c>
-      <c r="CA31" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="CB31" s="7" t="s">
-        <v>175</v>
+      <c r="CA31" s="32">
+        <f>223*(1+4.94%)</f>
+        <v>234.01620000000003</v>
+      </c>
+      <c r="CB31" s="32">
+        <f>1997*(1-7.13%)</f>
+        <v>1854.6138999999998</v>
       </c>
     </row>
     <row r="32" spans="1:80" ht="15.5" x14ac:dyDescent="0.35">
@@ -14972,8 +14978,9 @@
       <c r="BW53">
         <v>300</v>
       </c>
-      <c r="BX53" s="7" t="s">
-        <v>175</v>
+      <c r="BX53" s="7">
+        <f>858*(1+46%)</f>
+        <v>1252.68</v>
       </c>
       <c r="BY53">
         <v>655</v>
@@ -15981,23 +15988,29 @@
       <c r="BV57" s="4">
         <v>7</v>
       </c>
-      <c r="BW57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="BX57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="BY57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="BZ57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="CA57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="CB57" s="7" t="s">
-        <v>175</v>
+      <c r="BW57" s="24">
+        <f>250*(1+0.93%)</f>
+        <v>252.32500000000002</v>
+      </c>
+      <c r="BX57" s="24">
+        <f>294*(1+46%)</f>
+        <v>429.24</v>
+      </c>
+      <c r="BY57" s="24">
+        <f>264*(1-4.38%)</f>
+        <v>252.43680000000001</v>
+      </c>
+      <c r="BZ57" s="24">
+        <f>1098*(1+6.82%)</f>
+        <v>1172.8836000000001</v>
+      </c>
+      <c r="CA57" s="24">
+        <f>293*(1-4.94%)</f>
+        <v>278.5258</v>
+      </c>
+      <c r="CB57" s="24">
+        <f>1186*(1+7.13%)</f>
+        <v>1270.5617999999999</v>
       </c>
     </row>
     <row r="58" spans="1:180" ht="15.5" x14ac:dyDescent="0.35">
@@ -19566,7 +19579,8 @@
         <v>201.86</v>
       </c>
       <c r="BX71" s="24">
-        <v>528</v>
+        <f>528*(1+46%)</f>
+        <v>770.88</v>
       </c>
       <c r="BY71" s="21">
         <f>269*(1-4.38%)</f>
@@ -19836,7 +19850,8 @@
         <v>206.90650000000002</v>
       </c>
       <c r="BX72" s="21">
-        <v>473</v>
+        <f>473*(1+46%)</f>
+        <v>690.57999999999993</v>
       </c>
       <c r="BY72" s="21">
         <f>345*(1-4.38%)</f>
@@ -20108,7 +20123,8 @@
         <v>176.62750000000003</v>
       </c>
       <c r="BX73" s="21">
-        <v>171</v>
+        <f>171*(1+46%)</f>
+        <v>249.66</v>
       </c>
       <c r="BY73" s="21">
         <f>240*(1-4.38%)</f>
@@ -20380,7 +20396,8 @@
         <v>363.34800000000001</v>
       </c>
       <c r="BX74" s="24">
-        <v>378</v>
+        <f>378*(1+46%)</f>
+        <v>551.88</v>
       </c>
       <c r="BY74" s="21">
         <f>767*(1-4.38%)</f>
@@ -20652,7 +20669,8 @@
         <v>151.39500000000001</v>
       </c>
       <c r="BX75" s="24">
-        <v>275</v>
+        <f>275*(1+46%)</f>
+        <v>401.5</v>
       </c>
       <c r="BY75" s="21">
         <f>253*(1-4.38%)</f>
@@ -20924,7 +20942,8 @@
         <v>171.58100000000002</v>
       </c>
       <c r="BX76" s="21">
-        <v>789</v>
+        <f>789*(1+46%)</f>
+        <v>1151.94</v>
       </c>
       <c r="BY76" s="21">
         <f>330*(1-4.38%)</f>
@@ -21196,7 +21215,8 @@
         <v>191.76700000000002</v>
       </c>
       <c r="BX77" s="21">
-        <v>304</v>
+        <f>304*(1+46%)</f>
+        <v>443.84</v>
       </c>
       <c r="BY77" s="21">
         <f>168*(1-4.38%)</f>

</xml_diff>

<commit_message>
en siste endring? litt lei av R
</commit_message>
<xml_diff>
--- a/data/Revidert_resultatskjema.xlsx
+++ b/data/Revidert_resultatskjema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4138" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F42463B-51D3-46E1-A5BF-595DA409A7A2}"/>
+  <xr:revisionPtr revIDLastSave="4142" documentId="11_924805B546FA86936262E6F9983E8C1851038381" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA7C9F41-303C-4298-A981-17313C78A699}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="235">
   <si>
     <t>id</t>
   </si>
@@ -1193,9 +1193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD9" sqref="CD9"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CC77" sqref="CC77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -13748,11 +13748,11 @@
       <c r="CB47" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="CC47" s="32">
-        <v>1E-3</v>
-      </c>
-      <c r="CD47" s="32">
-        <v>1E-3</v>
+      <c r="CC47" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="CD47" s="32" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:82" ht="15.5" x14ac:dyDescent="0.35">
@@ -21698,7 +21698,8 @@
         <v>1117.3659</v>
       </c>
       <c r="CC77" s="2">
-        <v>2400.4</v>
+        <f>2400.4*(1-24.2%)</f>
+        <v>1819.5032000000001</v>
       </c>
       <c r="CD77" s="2">
         <f>835.2*(1+11%)</f>

</xml_diff>